<commit_message>
Output graphs and csvs generalised and tidied up
Finished generalising plotting options
Added more performance statistics and output as csv
Output all model results
Investigated effect of ODE rtol parameter on timings & quality of
output. Optimum around 0.001 to 0.05. Pick 0.01 (1%)
</commit_message>
<xml_diff>
--- a/notebooks/ModelInputs/parameters_v2.xlsx
+++ b/notebooks/ModelInputs/parameters_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="270" windowWidth="18195" windowHeight="11580"/>
+    <workbookView xWindow="480" yWindow="330" windowWidth="18195" windowHeight="11520"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="225">
   <si>
     <t>Param</t>
   </si>
@@ -470,211 +470,229 @@
     <t>Simulation end date. Format 'yyyy-mm-dd'</t>
   </si>
   <si>
+    <t>st_dt</t>
+  </si>
+  <si>
+    <t>end_dt</t>
+  </si>
+  <si>
+    <t>n_SC</t>
+  </si>
+  <si>
+    <t>Number of sub-catchments</t>
+  </si>
+  <si>
+    <t>Dynamic_EPC0</t>
+  </si>
+  <si>
+    <t>Calculate a dynamic soil water EPC0 (the equilibrium P concentration of zero sorption), so that it  varies with labile P content, or keep constant?</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Dynamic_effluent_inputs</t>
+  </si>
+  <si>
+    <t>Dynamic_terrestrialP_inputs</t>
+  </si>
+  <si>
+    <t>Dynamic_erodibility</t>
+  </si>
+  <si>
+    <t>Calculate within-year variability in soil erodibility due to crop management practices?</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Not yet implemented</t>
+  </si>
+  <si>
+    <t>inc_snowmelt</t>
+  </si>
+  <si>
+    <t>Include the snow accumulation and melt sub-module?</t>
+  </si>
+  <si>
+    <t>TDP_mg/l</t>
+  </si>
+  <si>
+    <t>TP_mg/l</t>
+  </si>
+  <si>
+    <t>If have TDP data:</t>
+  </si>
+  <si>
+    <t>If have TP data:</t>
+  </si>
+  <si>
+    <t>Areal soil mass calculation (kg/m2), Msoil_m2</t>
+  </si>
+  <si>
+    <t>This sheet provides some simple aides to parameterising the model. It is not read in to the model</t>
+  </si>
+  <si>
+    <t>M:\Working\NewModel\ModelInputs\Tar_AvMetData_1981-2010.csv</t>
+  </si>
+  <si>
+    <t>M:\Working\NewModel\ModelInputs\obs_csvs\Coull_9amDailyMeanQ_oldRating.xlsx</t>
+  </si>
+  <si>
+    <t>M:\Working\NewModel\ModelInputs\obs_csvs\WholePeriod\TarChem_R4_SS-P.xlsx</t>
+  </si>
+  <si>
+    <t>Only required if Dynamic_erodibility is set to 'y' in Setup parameters.</t>
+  </si>
+  <si>
+    <t>Only required if Dynamic_erodibility is set to 'y' in Setup parameters. e.g. 1st of March. Conversion from Calendar day to Julian day, see e.g. http://landweb.nascom.nasa.gov/browse/calendar.html</t>
+  </si>
+  <si>
+    <t>File paths for work desktop:</t>
+  </si>
+  <si>
+    <t>File paths for work laptop:</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Text; format 'yyyy-mm-dd'</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Text: cal or other (case sensitive)</t>
+  </si>
+  <si>
+    <t>Text: y or n (case sensitive)</t>
+  </si>
+  <si>
+    <t>output_fpath</t>
+  </si>
+  <si>
+    <t>File path to folder for model output to be written to (graphs and csvs)</t>
+  </si>
+  <si>
+    <t>plot_TC</t>
+  </si>
+  <si>
+    <t>plot_R</t>
+  </si>
+  <si>
+    <t>Save a plot of simulated output from the terrestrial compartment?</t>
+  </si>
+  <si>
+    <t>Save a plot of simulated output from the stream reaches?</t>
+  </si>
+  <si>
+    <t>List of reaches to plot reach output for</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>R_vars_to_plot</t>
+  </si>
+  <si>
+    <t>List of instream variables to plot</t>
+  </si>
+  <si>
+    <t>Choose from: SS, TDP, PP, TP, Q</t>
+  </si>
+  <si>
+    <t>output_figtype</t>
+  </si>
+  <si>
+    <t>File type for output figures to be saved as</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>Choose from: eps, jpg, pdf, pgf, png, ps, raw, rgba, svg, tif</t>
+  </si>
+  <si>
+    <t>output_fig_dpi</t>
+  </si>
+  <si>
+    <t>Resolution required for figures, in dpi</t>
+  </si>
+  <si>
+    <t>Integer, e.g. 150, 300, 600</t>
+  </si>
+  <si>
+    <t>Integer, e.g. 1</t>
+  </si>
+  <si>
+    <t>M:\Working\NewModel\ModelOutputs\Figs</t>
+  </si>
+  <si>
+    <t>plot_snow</t>
+  </si>
+  <si>
+    <t>If snow module included, plot results?</t>
+  </si>
+  <si>
+    <t>plot_reaches</t>
+  </si>
+  <si>
+    <t>Q, SS, TDP, PP, TP</t>
+  </si>
+  <si>
+    <t>plot_obs_style</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>Choose from: line, point (case sensitive)</t>
+  </si>
+  <si>
+    <t>Either list desired reaches (e.g. 1,2,10), or enter the word 'all' (case sensitive)</t>
+  </si>
+  <si>
+    <t>Plot reach timeseries in black &amp; white or colour?</t>
+  </si>
+  <si>
+    <t>colour_option</t>
+  </si>
+  <si>
+    <t>colour</t>
+  </si>
+  <si>
+    <t>Choose from: b&amp;w, colour</t>
+  </si>
+  <si>
+    <t>logy_list</t>
+  </si>
+  <si>
+    <t>SS, PP, TP</t>
+  </si>
+  <si>
+    <t>save_stats_csv</t>
+  </si>
+  <si>
+    <t>Output a csv of model performance statistics?</t>
+  </si>
+  <si>
+    <t>save_output_csvs</t>
+  </si>
+  <si>
+    <t>Output csvs of model results?</t>
+  </si>
+  <si>
+    <t>For reach plots, provide a list of variables for which y-axis is log-transformed. Mustn't include variables which aren't being plotted</t>
+  </si>
+  <si>
+    <t>How should the instream chemistry observations be plotted, as a line or as points? Discharge plotted as a line</t>
+  </si>
+  <si>
     <t>2004-01-01</t>
   </si>
   <si>
-    <t>st_dt</t>
-  </si>
-  <si>
-    <t>end_dt</t>
-  </si>
-  <si>
-    <t>n_SC</t>
-  </si>
-  <si>
-    <t>Number of sub-catchments</t>
-  </si>
-  <si>
-    <t>Dynamic_EPC0</t>
-  </si>
-  <si>
-    <t>Calculate a dynamic soil water EPC0 (the equilibrium P concentration of zero sorption), so that it  varies with labile P content, or keep constant?</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>Dynamic_effluent_inputs</t>
-  </si>
-  <si>
-    <t>Dynamic_terrestrialP_inputs</t>
-  </si>
-  <si>
-    <t>Dynamic_erodibility</t>
-  </si>
-  <si>
-    <t>Calculate within-year variability in soil erodibility due to crop management practices?</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>Not yet implemented</t>
-  </si>
-  <si>
-    <t>inc_snowmelt</t>
-  </si>
-  <si>
-    <t>Include the snow accumulation and melt sub-module?</t>
-  </si>
-  <si>
-    <t>TDP_mg/l</t>
-  </si>
-  <si>
-    <t>TP_mg/l</t>
-  </si>
-  <si>
-    <t>If have TDP data:</t>
-  </si>
-  <si>
-    <t>If have TP data:</t>
-  </si>
-  <si>
-    <t>Areal soil mass calculation (kg/m2), Msoil_m2</t>
-  </si>
-  <si>
-    <t>This sheet provides some simple aides to parameterising the model. It is not read in to the model</t>
-  </si>
-  <si>
-    <t>M:\Working\NewModel\ModelInputs\Tar_AvMetData_1981-2010.csv</t>
-  </si>
-  <si>
-    <t>M:\Working\NewModel\ModelInputs\obs_csvs\Coull_9amDailyMeanQ_oldRating.xlsx</t>
-  </si>
-  <si>
-    <t>M:\Working\NewModel\ModelInputs\obs_csvs\WholePeriod\TarChem_R4_SS-P.xlsx</t>
-  </si>
-  <si>
-    <t>Only required if Dynamic_erodibility is set to 'y' in Setup parameters.</t>
-  </si>
-  <si>
-    <t>Only required if Dynamic_erodibility is set to 'y' in Setup parameters. e.g. 1st of March. Conversion from Calendar day to Julian day, see e.g. http://landweb.nascom.nasa.gov/browse/calendar.html</t>
-  </si>
-  <si>
-    <t>File paths for work desktop:</t>
-  </si>
-  <si>
-    <t>File paths for work laptop:</t>
-  </si>
-  <si>
-    <t>Format</t>
-  </si>
-  <si>
-    <t>Text; format 'yyyy-mm-dd'</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Text: cal or other (case sensitive)</t>
-  </si>
-  <si>
-    <t>Text: y or n (case sensitive)</t>
-  </si>
-  <si>
-    <t>y or n (case sensitive)</t>
-  </si>
-  <si>
-    <t>output_fpath</t>
-  </si>
-  <si>
-    <t>File path to folder for model output to be written to (graphs and csvs)</t>
-  </si>
-  <si>
-    <t>plot_TC</t>
-  </si>
-  <si>
-    <t>plot_R</t>
-  </si>
-  <si>
-    <t>Save a plot of simulated output from the terrestrial compartment?</t>
-  </si>
-  <si>
-    <t>Save a plot of simulated output from the stream reaches?</t>
-  </si>
-  <si>
-    <t>List of reaches to plot reach output for</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>R_vars_to_plot</t>
-  </si>
-  <si>
-    <t>List of instream variables to plot</t>
-  </si>
-  <si>
-    <t>Choose from: SS, TDP, PP, TP, Q</t>
-  </si>
-  <si>
     <t>2004-12-31</t>
-  </si>
-  <si>
-    <t>output_figtype</t>
-  </si>
-  <si>
-    <t>File type for output figures to be saved as</t>
-  </si>
-  <si>
-    <t>png</t>
-  </si>
-  <si>
-    <t>Choose from: eps, jpg, pdf, pgf, png, ps, raw, rgba, svg, tif</t>
-  </si>
-  <si>
-    <t>output_fig_dpi</t>
-  </si>
-  <si>
-    <t>Resolution required for figures, in dpi</t>
-  </si>
-  <si>
-    <t>Integer, e.g. 150, 300, 600</t>
-  </si>
-  <si>
-    <t>Integer, e.g. 1</t>
-  </si>
-  <si>
-    <t>M:\Working\NewModel\ModelOutputs\Figs</t>
-  </si>
-  <si>
-    <t>plot_snow</t>
-  </si>
-  <si>
-    <t>If snow module included, plot results?</t>
-  </si>
-  <si>
-    <t>plot_reaches</t>
-  </si>
-  <si>
-    <t>Q, SS, TDP, PP, TP</t>
-  </si>
-  <si>
-    <t>plot_obs_style</t>
-  </si>
-  <si>
-    <t>line</t>
-  </si>
-  <si>
-    <t>Choose from: line, point (case sensitive)</t>
-  </si>
-  <si>
-    <t>Either list desired reaches (e.g. 1,2,10), or enter the word 'all' (case sensitive)</t>
-  </si>
-  <si>
-    <t>How should the chemistry observations be plotted, as a line or as points? Discharge obs automatically plotted as a line</t>
-  </si>
-  <si>
-    <t>Plot reach timeseries in black &amp; white or colour?</t>
-  </si>
-  <si>
-    <t>colour_option</t>
-  </si>
-  <si>
-    <t>Choose from: b&amp;w, colour (exactly reproduced)</t>
-  </si>
-  <si>
-    <t>colour</t>
   </si>
 </sst>
 </file>
@@ -956,7 +974,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1089,19 +1107,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1148,57 +1154,65 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1501,333 +1515,375 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="105" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.85546875" style="105" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="105" customWidth="1"/>
-    <col min="4" max="4" width="71.42578125" style="105" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="105"/>
+    <col min="1" max="1" width="26.7109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" style="102" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" style="102" customWidth="1"/>
+    <col min="4" max="4" width="53.5703125" style="102" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="102"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="56" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:4" s="107" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="105" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="109" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="102" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="99" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="102" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="99" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="108" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="109" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="102" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="99" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="108" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="109" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="102" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" s="99" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="108" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="109" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="102" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="99" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="108" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="109" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="102" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="99" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="108" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="109" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="103" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="99" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="103" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="104" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" s="105" t="s">
-        <v>172</v>
-      </c>
-      <c r="D2" s="106" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="103" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" s="104" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="105" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" s="107" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
-        <v>140</v>
-      </c>
-      <c r="B4" s="104" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="105" t="s">
-        <v>174</v>
-      </c>
-      <c r="D4" s="107" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="103" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" s="109" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="103" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="99" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="108" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="109" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="102">
+        <v>1</v>
+      </c>
+      <c r="D10" s="99" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="108" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="102" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="115" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="108" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="109" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="102" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" s="115" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="110" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="111"/>
+      <c r="C13" s="101" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="112"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="110" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" s="111"/>
+      <c r="C14" s="101" t="s">
+        <v>162</v>
+      </c>
+      <c r="D14" s="112"/>
+    </row>
+    <row r="15" spans="1:4" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="113" t="s">
+        <v>219</v>
+      </c>
+      <c r="B15" s="114" t="s">
+        <v>220</v>
+      </c>
+      <c r="C15" s="100" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="115" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="113" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="114" t="s">
+        <v>218</v>
+      </c>
+      <c r="C16" s="100" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="115" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="113" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" s="114" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="100" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="115" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="100" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="113" t="s">
         <v>185</v>
       </c>
-      <c r="B5" s="104" t="s">
+      <c r="B18" s="114" t="s">
+        <v>187</v>
+      </c>
+      <c r="C18" s="100" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" s="115" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="108" t="s">
         <v>186</v>
       </c>
-      <c r="C5" s="105" t="s">
+      <c r="B19" s="114" t="s">
+        <v>188</v>
+      </c>
+      <c r="C19" s="102" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="115" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="108" t="s">
+        <v>194</v>
+      </c>
+      <c r="B20" s="99" t="s">
+        <v>195</v>
+      </c>
+      <c r="C20" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" s="116" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="99" t="s">
+        <v>199</v>
+      </c>
+      <c r="C21" s="102">
+        <v>300</v>
+      </c>
+      <c r="D21" s="99" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="108" t="s">
         <v>205</v>
       </c>
-      <c r="D5" s="107" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="103" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" s="104" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="108" t="s">
-        <v>147</v>
-      </c>
-      <c r="D6" s="107" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7" s="104" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" s="108" t="s">
-        <v>157</v>
-      </c>
-      <c r="D7" s="107" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="103" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" s="104" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8" s="109" t="s">
-        <v>150</v>
-      </c>
-      <c r="D8" s="107" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="103" t="s">
-        <v>152</v>
-      </c>
-      <c r="B9" s="104" t="s">
-        <v>149</v>
-      </c>
-      <c r="C9" s="109" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" s="107" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="103" t="s">
-        <v>153</v>
-      </c>
-      <c r="B10" s="104" t="s">
-        <v>154</v>
-      </c>
-      <c r="C10" s="108">
-        <v>1</v>
-      </c>
-      <c r="D10" s="107" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="103" t="s">
-        <v>155</v>
-      </c>
-      <c r="B11" s="104" t="s">
-        <v>156</v>
-      </c>
-      <c r="C11" s="108" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="107" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="103" t="s">
-        <v>160</v>
-      </c>
-      <c r="B12" s="104" t="s">
-        <v>161</v>
-      </c>
-      <c r="C12" s="108" t="s">
-        <v>162</v>
-      </c>
-      <c r="D12" s="107" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="116" t="s">
-        <v>158</v>
-      </c>
-      <c r="B13" s="117"/>
-      <c r="C13" s="118" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="116"/>
-    </row>
-    <row r="14" spans="1:4" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="116" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" s="117"/>
-      <c r="C14" s="118" t="s">
-        <v>163</v>
-      </c>
-      <c r="D14" s="116"/>
-    </row>
-    <row r="15" spans="1:4" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="110" t="s">
+      <c r="B22" s="99" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="102" t="s">
+        <v>190</v>
+      </c>
+      <c r="D22" s="116" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="108" t="s">
+        <v>191</v>
+      </c>
+      <c r="B23" s="99" t="s">
+        <v>192</v>
+      </c>
+      <c r="C23" s="102" t="s">
         <v>206</v>
       </c>
-      <c r="B15" s="111" t="s">
+      <c r="D23" s="116" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="108" t="s">
         <v>207</v>
       </c>
-      <c r="C15" s="112" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" s="110" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="113" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="110" t="s">
-        <v>187</v>
-      </c>
-      <c r="B16" s="111" t="s">
-        <v>189</v>
-      </c>
-      <c r="C16" s="112" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="110" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="105" t="s">
-        <v>188</v>
-      </c>
-      <c r="B17" s="111" t="s">
-        <v>190</v>
-      </c>
-      <c r="C17" s="105" t="s">
-        <v>157</v>
-      </c>
-      <c r="D17" s="110" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="105" t="s">
+      <c r="B24" s="109" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" s="102" t="s">
         <v>208</v>
       </c>
-      <c r="B18" s="105" t="s">
-        <v>191</v>
-      </c>
-      <c r="C18" s="105" t="s">
-        <v>192</v>
-      </c>
-      <c r="D18" s="114" t="s">
+      <c r="D24" s="116" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="108" t="s">
+        <v>212</v>
+      </c>
+      <c r="B25" s="109" t="s">
+        <v>211</v>
+      </c>
+      <c r="C25" s="102" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="105" t="s">
+      <c r="D25" s="116" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="B26" s="117" t="s">
+        <v>221</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="D26" s="118" t="s">
         <v>193</v>
-      </c>
-      <c r="B19" s="105" t="s">
-        <v>194</v>
-      </c>
-      <c r="C19" s="105" t="s">
-        <v>209</v>
-      </c>
-      <c r="D19" s="114" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="105" t="s">
-        <v>210</v>
-      </c>
-      <c r="B20" s="120" t="s">
-        <v>214</v>
-      </c>
-      <c r="C20" s="105" t="s">
-        <v>211</v>
-      </c>
-      <c r="D20" s="114" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="105" t="s">
-        <v>216</v>
-      </c>
-      <c r="B21" s="120" t="s">
-        <v>215</v>
-      </c>
-      <c r="C21" s="105" t="s">
-        <v>218</v>
-      </c>
-      <c r="D21" s="114" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="105" t="s">
-        <v>197</v>
-      </c>
-      <c r="B22" s="105" t="s">
-        <v>198</v>
-      </c>
-      <c r="C22" s="105" t="s">
-        <v>199</v>
-      </c>
-      <c r="D22" s="115" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="105" t="s">
-        <v>201</v>
-      </c>
-      <c r="B23" s="105" t="s">
-        <v>202</v>
-      </c>
-      <c r="C23" s="11">
-        <v>300</v>
-      </c>
-      <c r="D23" s="105" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -1853,181 +1909,181 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="72" t="s">
+      <c r="G1" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="73" t="s">
+      <c r="I1" s="69" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="80">
+      <c r="E2" s="76">
         <v>2</v>
       </c>
-      <c r="F2" s="81">
+      <c r="F2" s="77">
         <v>7</v>
       </c>
-      <c r="G2" s="82"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="84"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="80"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="81" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="86" t="s">
+      <c r="D3" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="E3" s="87">
+      <c r="E3" s="83">
         <v>1100</v>
       </c>
-      <c r="F3" s="88">
+      <c r="F3" s="84">
         <v>900</v>
       </c>
-      <c r="G3" s="89"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="91"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="87"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="74">
+      <c r="E4" s="70">
         <v>10</v>
       </c>
-      <c r="F4" s="66">
+      <c r="F4" s="62">
         <v>0</v>
       </c>
-      <c r="G4" s="64"/>
-      <c r="H4" s="76">
+      <c r="G4" s="60"/>
+      <c r="H4" s="72">
         <v>-3</v>
       </c>
-      <c r="I4" s="65" t="s">
+      <c r="I4" s="61" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="92">
+      <c r="E5" s="88">
         <v>0.12</v>
       </c>
-      <c r="F5" s="93">
+      <c r="F5" s="89">
         <v>0</v>
       </c>
-      <c r="G5" s="69"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="70" t="s">
+      <c r="G5" s="65"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="66" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="59" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="62">
+      <c r="E6" s="58">
         <v>0.2</v>
       </c>
-      <c r="F6" s="63">
+      <c r="F6" s="59">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G6" s="63">
+      <c r="G6" s="59">
         <v>0.09</v>
       </c>
-      <c r="H6" s="75"/>
-      <c r="I6" s="65"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="61"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="64" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="D7" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="67">
+      <c r="E7" s="63">
         <v>0</v>
       </c>
-      <c r="F7" s="68">
+      <c r="F7" s="64">
         <v>0</v>
       </c>
-      <c r="G7" s="68">
+      <c r="G7" s="64">
         <v>0</v>
       </c>
-      <c r="H7" s="77"/>
-      <c r="I7" s="70"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="66"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2040,7 +2096,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E5" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,274 +2107,274 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="96">
+      <c r="E1" s="92">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="101">
+      <c r="E2" s="97">
         <v>51.7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="E3" s="97">
+      <c r="E3" s="93">
         <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="97">
+      <c r="E4" s="93">
         <v>0.3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="97">
+      <c r="E5" s="93">
         <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="90" t="s">
         <v>92</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="97">
+      <c r="E6" s="93">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="94" t="s">
+      <c r="B7" s="90" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="E7" s="97">
+      <c r="E7" s="93">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="94" t="s">
+      <c r="B8" s="90" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="97">
+      <c r="E8" s="93">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="90" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="E9" s="97">
+      <c r="E9" s="93">
         <v>0.65</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="94" t="s">
+      <c r="B10" s="90" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="E10" s="98">
+      <c r="E10" s="94">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="94" t="s">
+      <c r="B11" s="90" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="E11" s="98">
+      <c r="E11" s="94">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="62" t="s">
+      <c r="A12" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="94" t="s">
+      <c r="B12" s="90" t="s">
         <v>126</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="98">
+      <c r="E12" s="94">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="67" t="s">
+      <c r="A13" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="95" t="s">
+      <c r="B13" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="68" t="s">
+      <c r="C13" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="68" t="s">
+      <c r="D13" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="102">
+      <c r="E13" s="98">
         <v>5000</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="85" t="s">
+      <c r="A14" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="100" t="s">
+      <c r="B14" s="96" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="D14" s="86" t="s">
+      <c r="D14" s="82" t="s">
         <v>113</v>
       </c>
-      <c r="E14" s="101">
+      <c r="E14" s="97">
         <v>2.4E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="68" t="s">
+      <c r="D15" s="64" t="s">
         <v>119</v>
       </c>
-      <c r="E15" s="102">
+      <c r="E15" s="98">
         <v>0.8</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="67" t="s">
+      <c r="A16" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="95" t="s">
+      <c r="B16" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="68" t="s">
+      <c r="C16" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="68" t="s">
+      <c r="D16" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="99">
+      <c r="E16" s="95">
         <v>0.26</v>
       </c>
     </row>
@@ -2333,7 +2389,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2671,7 +2727,7 @@
         <v>109</v>
       </c>
       <c r="E18" s="31">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="F18" s="37" t="s">
         <v>120</v>
@@ -2712,7 +2768,7 @@
         <v>60</v>
       </c>
       <c r="F20" s="54" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2732,7 +2788,7 @@
         <v>304</v>
       </c>
       <c r="F21" s="55" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2800,7 +2856,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2810,7 +2866,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2818,7 +2874,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>42</v>
@@ -2838,7 +2894,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2846,7 +2902,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>43</v>
@@ -2879,7 +2935,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2918,41 +2974,41 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="56" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="56" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="57" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="56" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="57" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="57" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="61" t="s">
+      <c r="A25" s="57" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="61" t="s">
+      <c r="A26" s="57" t="s">
         <v>144</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Small improvement to evapotranspiration calculation
Function linking AET and PET is now scaled according to field capacity,
rather than being hard-wired (mu, the scaling factor in the exponential,
is now calculated in the model rather than being constant at 0.02)
Also re-named f_IExcess throughout to f_quick, to make it explicit that
quick flow is not infiltration excess.
</commit_message>
<xml_diff>
--- a/notebooks/ModelInputs/parameters_v2.xlsx
+++ b/notebooks/ModelInputs/parameters_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="18195" windowHeight="11520"/>
+    <workbookView xWindow="480" yWindow="330" windowWidth="18195" windowHeight="11520" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -32,9 +32,6 @@
     <t>IG</t>
   </si>
   <si>
-    <t>f_IExcess</t>
-  </si>
-  <si>
     <t>fc</t>
   </si>
   <si>
@@ -693,6 +690,9 @@
   </si>
   <si>
     <t>2004-12-31</t>
+  </si>
+  <si>
+    <t>f_quick</t>
   </si>
 </sst>
 </file>
@@ -1517,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,355 +1535,355 @@
         <v>0</v>
       </c>
       <c r="B1" s="105" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="106" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="105" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="108" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="109" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="109" t="s">
-        <v>137</v>
-      </c>
       <c r="C2" s="102" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D2" s="99" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="109" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="109" t="s">
-        <v>139</v>
-      </c>
       <c r="C3" s="102" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D3" s="99" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="108" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="109" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="109" t="s">
-        <v>141</v>
-      </c>
       <c r="C4" s="102" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D4" s="99" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="108" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="109" t="s">
         <v>183</v>
       </c>
-      <c r="B5" s="109" t="s">
-        <v>184</v>
-      </c>
       <c r="C5" s="102" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D5" s="99" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="108" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="109" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="109" t="s">
+      <c r="C6" s="102" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="102" t="s">
-        <v>147</v>
-      </c>
       <c r="D6" s="99" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="108" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="109" t="s">
         <v>163</v>
       </c>
-      <c r="B7" s="109" t="s">
-        <v>164</v>
-      </c>
       <c r="C7" s="102" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D7" s="99" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="108" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B8" s="109" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" s="103" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8" s="99" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="108" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="109" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" s="103" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D9" s="99" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" s="109" t="s">
         <v>152</v>
-      </c>
-      <c r="B10" s="109" t="s">
-        <v>153</v>
       </c>
       <c r="C10" s="102">
         <v>1</v>
       </c>
       <c r="D10" s="99" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="108" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11" s="109" t="s">
         <v>154</v>
       </c>
-      <c r="B11" s="109" t="s">
-        <v>155</v>
-      </c>
       <c r="C11" s="102" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D11" s="115" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="108" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="109" t="s">
         <v>159</v>
       </c>
-      <c r="B12" s="109" t="s">
+      <c r="C12" s="102" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="102" t="s">
-        <v>161</v>
-      </c>
       <c r="D12" s="115" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="110" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B13" s="111"/>
       <c r="C13" s="101" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D13" s="112"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="110" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B14" s="111"/>
       <c r="C14" s="101" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D14" s="112"/>
     </row>
     <row r="15" spans="1:4" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="113" t="s">
+        <v>218</v>
+      </c>
+      <c r="B15" s="114" t="s">
         <v>219</v>
       </c>
-      <c r="B15" s="114" t="s">
-        <v>220</v>
-      </c>
       <c r="C15" s="100" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D15" s="115" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="113" t="s">
+        <v>216</v>
+      </c>
+      <c r="B16" s="114" t="s">
         <v>217</v>
       </c>
-      <c r="B16" s="114" t="s">
-        <v>218</v>
-      </c>
       <c r="C16" s="100" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D16" s="115" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="113" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" s="114" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="114" t="s">
-        <v>204</v>
-      </c>
       <c r="C17" s="100" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D17" s="115" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="100" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="113" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B18" s="114" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C18" s="100" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D18" s="115" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="108" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B19" s="114" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C19" s="102" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D19" s="115" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="108" t="s">
+        <v>193</v>
+      </c>
+      <c r="B20" s="99" t="s">
         <v>194</v>
       </c>
-      <c r="B20" s="99" t="s">
+      <c r="C20" s="102" t="s">
         <v>195</v>
       </c>
-      <c r="C20" s="102" t="s">
+      <c r="D20" s="116" t="s">
         <v>196</v>
-      </c>
-      <c r="D20" s="116" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="108" t="s">
+        <v>197</v>
+      </c>
+      <c r="B21" s="99" t="s">
         <v>198</v>
-      </c>
-      <c r="B21" s="99" t="s">
-        <v>199</v>
       </c>
       <c r="C21" s="102">
         <v>300</v>
       </c>
       <c r="D21" s="99" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="108" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B22" s="99" t="s">
+        <v>188</v>
+      </c>
+      <c r="C22" s="102" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="102" t="s">
-        <v>190</v>
-      </c>
       <c r="D22" s="116" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="108" t="s">
+        <v>190</v>
+      </c>
+      <c r="B23" s="99" t="s">
         <v>191</v>
       </c>
-      <c r="B23" s="99" t="s">
+      <c r="C23" s="102" t="s">
+        <v>205</v>
+      </c>
+      <c r="D23" s="116" t="s">
         <v>192</v>
-      </c>
-      <c r="C23" s="102" t="s">
-        <v>206</v>
-      </c>
-      <c r="D23" s="116" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="108" t="s">
+        <v>206</v>
+      </c>
+      <c r="B24" s="109" t="s">
+        <v>221</v>
+      </c>
+      <c r="C24" s="102" t="s">
         <v>207</v>
       </c>
-      <c r="B24" s="109" t="s">
-        <v>222</v>
-      </c>
-      <c r="C24" s="102" t="s">
+      <c r="D24" s="116" t="s">
         <v>208</v>
-      </c>
-      <c r="D24" s="116" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="108" t="s">
+        <v>211</v>
+      </c>
+      <c r="B25" s="109" t="s">
+        <v>210</v>
+      </c>
+      <c r="C25" s="102" t="s">
         <v>212</v>
       </c>
-      <c r="B25" s="109" t="s">
-        <v>211</v>
-      </c>
-      <c r="C25" s="102" t="s">
+      <c r="D25" s="116" t="s">
         <v>213</v>
-      </c>
-      <c r="D25" s="116" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="B26" s="117" t="s">
+        <v>220</v>
+      </c>
+      <c r="C26" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="B26" s="117" t="s">
-        <v>221</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>216</v>
-      </c>
       <c r="D26" s="118" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -1910,16 +1910,16 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="68" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="68" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="67" t="s">
         <v>1</v>
@@ -1931,24 +1931,24 @@
         <v>3</v>
       </c>
       <c r="H1" s="69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I1" s="69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="75" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="75" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="76">
         <v>2</v>
@@ -1962,16 +1962,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="81" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="82" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="82" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E3" s="83">
         <v>1100</v>
@@ -1985,16 +1985,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E4" s="70">
         <v>10</v>
@@ -2007,21 +2007,21 @@
         <v>-3</v>
       </c>
       <c r="I4" s="61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="64" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="88">
         <v>0.12</v>
@@ -2032,21 +2032,21 @@
       <c r="G5" s="65"/>
       <c r="H5" s="73"/>
       <c r="I5" s="66" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" s="58">
         <v>0.2</v>
@@ -2062,16 +2062,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="64" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C7" s="64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E7" s="63">
         <v>0</v>
@@ -2108,16 +2108,16 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="68" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="68" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="92">
         <v>1</v>
@@ -2125,16 +2125,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="96" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="82" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="82" t="s">
         <v>50</v>
-      </c>
-      <c r="D2" s="82" t="s">
-        <v>51</v>
       </c>
       <c r="E2" s="97">
         <v>51.7</v>
@@ -2142,16 +2142,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="90" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="93">
         <v>0.2</v>
@@ -2159,16 +2159,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="90" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E4" s="93">
         <v>0.3</v>
@@ -2176,16 +2176,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="90" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="93">
         <v>0.5</v>
@@ -2193,16 +2193,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="90" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E6" s="93">
         <v>0</v>
@@ -2210,16 +2210,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="90" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="59" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E7" s="93">
         <v>0</v>
@@ -2227,16 +2227,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="90" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="59" t="s">
         <v>94</v>
-      </c>
-      <c r="C8" s="59" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="59" t="s">
-        <v>95</v>
       </c>
       <c r="E8" s="93">
         <v>0</v>
@@ -2244,16 +2244,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="90" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="59" t="s">
         <v>123</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="59" t="s">
-        <v>124</v>
       </c>
       <c r="E9" s="93">
         <v>0.65</v>
@@ -2261,16 +2261,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="90" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E10" s="94">
         <v>4</v>
@@ -2278,16 +2278,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="90" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="59" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E11" s="94">
         <v>4</v>
@@ -2295,16 +2295,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="90" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" s="59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="59" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E12" s="94">
         <v>10</v>
@@ -2312,16 +2312,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13" s="91" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="98">
         <v>5000</v>
@@ -2329,16 +2329,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="96" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="82" t="s">
+      <c r="D14" s="82" t="s">
         <v>112</v>
-      </c>
-      <c r="D14" s="82" t="s">
-        <v>113</v>
       </c>
       <c r="E14" s="97">
         <v>2.4E-2</v>
@@ -2346,16 +2346,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="91" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="64" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="64" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E15" s="98">
         <v>0.8</v>
@@ -2363,16 +2363,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="63" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" s="91" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" s="95">
         <v>0.26</v>
@@ -2388,8 +2388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2405,36 +2405,36 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>131</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>132</v>
       </c>
       <c r="E2" s="22">
         <v>0</v>
@@ -2443,16 +2443,16 @@
     </row>
     <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="D3" s="25" t="s">
         <v>134</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>135</v>
       </c>
       <c r="E3" s="25">
         <v>2.74</v>
@@ -2461,16 +2461,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>4</v>
+        <v>224</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="44">
         <v>1.4999999999999999E-2</v>
@@ -2479,16 +2479,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="33">
         <v>0.95</v>
@@ -2497,16 +2497,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="34">
         <v>290</v>
@@ -2515,16 +2515,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="33">
         <v>0.6</v>
@@ -2533,16 +2533,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="34">
         <v>65</v>
@@ -2551,16 +2551,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="31" t="s">
         <v>59</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>60</v>
       </c>
       <c r="E9" s="35">
         <v>0.4</v>
@@ -2569,16 +2569,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="31" t="s">
         <v>61</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>62</v>
       </c>
       <c r="E10" s="35">
         <v>0.5</v>
@@ -2587,16 +2587,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E11" s="35">
         <v>0.5</v>
@@ -2605,16 +2605,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="35">
         <v>1</v>
@@ -2623,16 +2623,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="40">
         <v>1</v>
@@ -2641,16 +2641,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="43" t="s">
         <v>67</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>68</v>
       </c>
       <c r="E14" s="46">
         <v>200</v>
@@ -2659,36 +2659,36 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E15" s="36">
         <v>3.2237299999999997E-5</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E16" s="47">
         <v>1.4999999999999999E-2</v>
@@ -2697,16 +2697,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" s="50">
         <v>2</v>
@@ -2715,36 +2715,36 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E18" s="31">
         <v>30</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E19" s="35">
         <v>1.2</v>
@@ -2753,56 +2753,56 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20" s="53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E20" s="53">
         <v>60</v>
       </c>
       <c r="F20" s="54" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" s="53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C21" s="53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E21" s="53">
         <v>304</v>
       </c>
       <c r="F21" s="55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E22" s="34">
         <v>250</v>
@@ -2811,16 +2811,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E23" s="40">
         <v>1.7</v>
@@ -2856,28 +2856,28 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>41</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2894,24 +2894,24 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>41</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2935,81 +2935,81 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="14">
         <v>1000</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="5">
         <v>20</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" s="17">
         <f>B14*B15/100</f>
         <v>200</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="57" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New hydrology notebook exploring options
New notebook exploring & plotting the various hydrology options explored
during model development
</commit_message>
<xml_diff>
--- a/notebooks/ModelInputs/parameters_v2.xlsx
+++ b/notebooks/ModelInputs/parameters_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="18195" windowHeight="11520" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="330" windowWidth="18195" windowHeight="11520"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -635,9 +635,6 @@
     <t>plot_reaches</t>
   </si>
   <si>
-    <t>Q, SS, TDP, PP, TP</t>
-  </si>
-  <si>
     <t>plot_obs_style</t>
   </si>
   <si>
@@ -680,19 +677,22 @@
     <t>Output csvs of model results?</t>
   </si>
   <si>
-    <t>For reach plots, provide a list of variables for which y-axis is log-transformed. Mustn't include variables which aren't being plotted</t>
-  </si>
-  <si>
     <t>How should the instream chemistry observations be plotted, as a line or as points? Discharge plotted as a line</t>
   </si>
   <si>
     <t>2004-01-01</t>
   </si>
   <si>
-    <t>2004-12-31</t>
-  </si>
-  <si>
     <t>f_quick</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>2005-12-31</t>
+  </si>
+  <si>
+    <t>For reach plots, provide a list of variables for which y-axis is log-transformed</t>
   </si>
 </sst>
 </file>
@@ -1517,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,7 +1636,7 @@
         <v>147</v>
       </c>
       <c r="C8" s="103" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D8" s="99" t="s">
         <v>178</v>
@@ -1720,10 +1720,10 @@
     </row>
     <row r="15" spans="1:4" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="113" t="s">
+        <v>217</v>
+      </c>
+      <c r="B15" s="114" t="s">
         <v>218</v>
-      </c>
-      <c r="B15" s="114" t="s">
-        <v>219</v>
       </c>
       <c r="C15" s="100" t="s">
         <v>160</v>
@@ -1734,10 +1734,10 @@
     </row>
     <row r="16" spans="1:4" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="113" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16" s="114" t="s">
         <v>216</v>
-      </c>
-      <c r="B16" s="114" t="s">
-        <v>217</v>
       </c>
       <c r="C16" s="100" t="s">
         <v>160</v>
@@ -1768,7 +1768,7 @@
         <v>186</v>
       </c>
       <c r="C18" s="100" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D18" s="115" t="s">
         <v>181</v>
@@ -1827,7 +1827,7 @@
         <v>189</v>
       </c>
       <c r="D22" s="116" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1838,7 +1838,7 @@
         <v>191</v>
       </c>
       <c r="C23" s="102" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="D23" s="116" t="s">
         <v>192</v>
@@ -1846,41 +1846,41 @@
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="108" t="s">
+        <v>205</v>
+      </c>
+      <c r="B24" s="109" t="s">
+        <v>219</v>
+      </c>
+      <c r="C24" s="102" t="s">
         <v>206</v>
       </c>
-      <c r="B24" s="109" t="s">
-        <v>221</v>
-      </c>
-      <c r="C24" s="102" t="s">
+      <c r="D24" s="116" t="s">
         <v>207</v>
-      </c>
-      <c r="D24" s="116" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="108" t="s">
+        <v>210</v>
+      </c>
+      <c r="B25" s="109" t="s">
+        <v>209</v>
+      </c>
+      <c r="C25" s="102" t="s">
         <v>211</v>
       </c>
-      <c r="B25" s="109" t="s">
-        <v>210</v>
-      </c>
-      <c r="C25" s="102" t="s">
+      <c r="D25" s="116" t="s">
         <v>212</v>
       </c>
-      <c r="D25" s="116" t="s">
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+      <c r="B26" s="117" t="s">
+        <v>224</v>
+      </c>
+      <c r="C26" s="25" t="s">
         <v>214</v>
-      </c>
-      <c r="B26" s="117" t="s">
-        <v>220</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>215</v>
       </c>
       <c r="D26" s="118" t="s">
         <v>192</v>
@@ -2388,8 +2388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2464,7 +2464,7 @@
         <v>81</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C4" s="43" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Option to plot dynamic crop cover factor
Plus a couple of other small changes
</commit_message>
<xml_diff>
--- a/notebooks/ModelInputs/parameters_v2.xlsx
+++ b/notebooks/ModelInputs/parameters_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="18195" windowHeight="11520"/>
+    <workbookView xWindow="480" yWindow="330" windowWidth="18195" windowHeight="11520" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -110,589 +110,589 @@
     <t>Qg_min</t>
   </si>
   <si>
+    <t>Qg0_init</t>
+  </si>
+  <si>
+    <t>Qr0_init</t>
+  </si>
+  <si>
+    <t>E_Q</t>
+  </si>
+  <si>
+    <t>k_EQ</t>
+  </si>
+  <si>
+    <t>TDPeff</t>
+  </si>
+  <si>
+    <t>TDPg</t>
+  </si>
+  <si>
+    <t>E_PP</t>
+  </si>
+  <si>
+    <t>Msoil_m2</t>
+  </si>
+  <si>
+    <t>Q_m3/s</t>
+  </si>
+  <si>
+    <t>TDP_kg/day</t>
+  </si>
+  <si>
+    <t>fraction as TDP</t>
+  </si>
+  <si>
+    <t>TP_kg/day</t>
+  </si>
+  <si>
+    <t>Template for calculating daily sewage fluxes to the stream (kg P/day as PP or TDP), from known effluent discharge and P concentration</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Soil water time constant</t>
+  </si>
+  <si>
+    <t>Proportion of precipitation that contributes to quick flow</t>
+  </si>
+  <si>
+    <t>PET reduction factor</t>
+  </si>
+  <si>
+    <t>km2</t>
+  </si>
+  <si>
+    <t>Catchment area</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>degrees</t>
+  </si>
+  <si>
+    <t>kg/day</t>
+  </si>
+  <si>
+    <t>Reach length</t>
+  </si>
+  <si>
+    <t>Reach effluent TDP inputs</t>
+  </si>
+  <si>
+    <t>Baseflow index</t>
+  </si>
+  <si>
+    <t>Groundwater time constant</t>
+  </si>
+  <si>
+    <t>mm/d</t>
+  </si>
+  <si>
+    <t>Minimum groundwater flow</t>
+  </si>
+  <si>
+    <t>1/m3</t>
+  </si>
+  <si>
+    <t>Gradient of stream velocity-discharge relationship</t>
+  </si>
+  <si>
+    <t>Exponent of stream velocity-discharge relationship</t>
+  </si>
+  <si>
+    <t>Initial groundwater flow</t>
+  </si>
+  <si>
+    <t>Initial in-stream flow</t>
+  </si>
+  <si>
+    <t>m3/s</t>
+  </si>
+  <si>
+    <t>kg/m2</t>
+  </si>
+  <si>
+    <t>Soil mass per m2</t>
+  </si>
+  <si>
+    <t>Soil bulk density</t>
+  </si>
+  <si>
+    <t>Soil depth</t>
+  </si>
+  <si>
+    <t>Soil mass/m2</t>
+  </si>
+  <si>
+    <t>kg/m3</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>Particulate P enrichment factor</t>
+  </si>
+  <si>
+    <t>Groundwater TDP concentration</t>
+  </si>
+  <si>
+    <t>Instream entrainment factor</t>
+  </si>
+  <si>
+    <t>Instream entrainment non-linear coefficient</t>
+  </si>
+  <si>
+    <t>Soil field capacity</t>
+  </si>
+  <si>
+    <t>mm/kg soil</t>
+  </si>
+  <si>
+    <t>Terrestrial sediment delivery non-linear coefficient</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Hydrology</t>
+  </si>
+  <si>
+    <t>Dissolved P</t>
+  </si>
+  <si>
+    <t>Particulate P</t>
+  </si>
+  <si>
+    <t>Sediment</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>T_s</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Initial soil water EPC0, in mg/l</t>
+  </si>
+  <si>
+    <t>Semi-natural fixed</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>f_NC_Ar</t>
+  </si>
+  <si>
+    <t>f_NC_IG</t>
+  </si>
+  <si>
+    <t>f_NC_S</t>
+  </si>
+  <si>
+    <t>Proportion of newly-converted SN (from agricultural). If have newly-converted IG or Ar, this must be 0</t>
+  </si>
+  <si>
+    <t>Proportion of newly-converted arable land (from SN). If f_NC_S&gt;0, this must be 0</t>
+  </si>
+  <si>
+    <t>Proportion of newly-converted IG (from SN). If f_NC_S&gt;0, this must be 0</t>
+  </si>
+  <si>
+    <t>Semi-natural fixed at 0. Newly-converted value could be negative if have net uptake.</t>
+  </si>
+  <si>
+    <t>Net annual P input to the soil (may be negative if have more uptake than input)</t>
+  </si>
+  <si>
+    <t>A value only needs to be supplied when the model is run in validation mode. In calibration mode, it is calculated within the model and output as Kf</t>
+  </si>
+  <si>
+    <t>Proportion of arable land, excluding any newly-converted from SN</t>
+  </si>
+  <si>
+    <t>Proportion of improved grassland, excluding any newly-converted from SN</t>
+  </si>
+  <si>
+    <t>Proportion of semi-natural and other low soil-P land, excluding any newly-converted from agricultural</t>
+  </si>
+  <si>
+    <t>S_Ar</t>
+  </si>
+  <si>
+    <t>S_IG</t>
+  </si>
+  <si>
+    <t>Mean slope of arable land in the sub-catchment</t>
+  </si>
+  <si>
+    <t>Mean slope of improved grassland in the sub-catchment</t>
+  </si>
+  <si>
+    <t>Mean slope of semi-natural land in the sub-catchment</t>
+  </si>
+  <si>
+    <t>Scaling factor for soil yield to the stream</t>
+  </si>
+  <si>
+    <t>m s2/kg</t>
+  </si>
+  <si>
+    <t>K_erosion</t>
+  </si>
+  <si>
+    <t>T/ha</t>
+  </si>
+  <si>
+    <t>Inherent soil erodibility, averaged for soils over the sub-catchment. Derived e.g. from http://esdac.jrc.ec.europa.eu/themes/soil-erodibility-europe</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>d_maxE_spr</t>
+  </si>
+  <si>
+    <t>d_maxE_aut</t>
+  </si>
+  <si>
+    <t>Day of the year when soil erodibility is at its maximum for spring-sown crops</t>
+  </si>
+  <si>
+    <t>Day of the year when soil erodibility is at its maximum for autumn-sown crops</t>
+  </si>
+  <si>
+    <t>Reach slope (ideally length-weighted)</t>
+  </si>
+  <si>
+    <t>Incorporates connectivity. May therefore need to change per sub-catchment</t>
+  </si>
+  <si>
+    <t>Vegetation cover factor, describing ratio between long-term erosion under the land use class, compared to under bare soil of the same soil type, slope, etc. Sourced from (R)USLE literature.</t>
+  </si>
+  <si>
+    <t>C_cover</t>
+  </si>
+  <si>
+    <t>f_spr</t>
+  </si>
+  <si>
+    <t>Proportion spring-sown crops make to total arable land area (assume rest is autumn-sown)</t>
+  </si>
+  <si>
+    <t>Sed_measures</t>
+  </si>
+  <si>
+    <t>S_SN</t>
+  </si>
+  <si>
+    <t>Reduction in load of sediment delivered to the stream (proportion; 0-1) due to management measures, e.g. buffer strips, filter fences, conservation tillage practices, etc.)</t>
+  </si>
+  <si>
+    <t>Phosphorus sorption coefficient (gradient of linear relationship between labile P and TDP concentration)</t>
+  </si>
+  <si>
+    <t>Initial total soil P content. If you only have 'labile P' data, calculate this using your assumed ratio for the connection between total and labile soil P masses ('k_labile' in 'constant' parameters)</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>D_snow_0</t>
+  </si>
+  <si>
+    <t>Initial snow depth in the catchment</t>
+  </si>
+  <si>
+    <t>f_DDSM</t>
+  </si>
+  <si>
+    <t>mm/(degree-day deg C)</t>
+  </si>
+  <si>
+    <t>Degree-day factor for snow melt</t>
+  </si>
+  <si>
+    <t>metdata_fpath</t>
+  </si>
+  <si>
+    <t>File path to input meteorological data file</t>
+  </si>
+  <si>
+    <t>Qobsdata_fpath</t>
+  </si>
+  <si>
+    <t>File path to discharge observations</t>
+  </si>
+  <si>
+    <t>chemObsData_fpath</t>
+  </si>
+  <si>
+    <t>File path to chemistry observations</t>
+  </si>
+  <si>
+    <t>C:\Users\lj40184\Documents\GitHub\enviro_mod_notes\notebooks\ModelInputs\Tar_AvMetData_1981-2010.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\lj40184\Documents\GitHub\enviro_mod_notes\notebooks\ModelInputs\obs_csvs\Coull_9amDailyMeanQ_oldRating.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\lj40184\Documents\GitHub\enviro_mod_notes\notebooks\ModelInputs\obs_csvs\WholePeriod\TarChem_R4_SS-P.xlsx</t>
+  </si>
+  <si>
+    <t>run_mode</t>
+  </si>
+  <si>
+    <t>One of 'cal', 'other'. Determines whether the soil sorption coefficient, Kf, is calculated (calibration period) or read in as a parameter</t>
+  </si>
+  <si>
+    <t>cal</t>
+  </si>
+  <si>
+    <t>Simulation start date</t>
+  </si>
+  <si>
+    <t>Simulation end date. Format 'yyyy-mm-dd'</t>
+  </si>
+  <si>
+    <t>st_dt</t>
+  </si>
+  <si>
+    <t>end_dt</t>
+  </si>
+  <si>
+    <t>n_SC</t>
+  </si>
+  <si>
+    <t>Number of sub-catchments</t>
+  </si>
+  <si>
+    <t>Dynamic_EPC0</t>
+  </si>
+  <si>
+    <t>Calculate a dynamic soil water EPC0 (the equilibrium P concentration of zero sorption), so that it  varies with labile P content, or keep constant?</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Dynamic_effluent_inputs</t>
+  </si>
+  <si>
+    <t>Dynamic_terrestrialP_inputs</t>
+  </si>
+  <si>
+    <t>Dynamic_erodibility</t>
+  </si>
+  <si>
+    <t>Calculate within-year variability in soil erodibility due to crop management practices?</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Not yet implemented</t>
+  </si>
+  <si>
+    <t>inc_snowmelt</t>
+  </si>
+  <si>
+    <t>Include the snow accumulation and melt sub-module?</t>
+  </si>
+  <si>
+    <t>TDP_mg/l</t>
+  </si>
+  <si>
+    <t>TP_mg/l</t>
+  </si>
+  <si>
+    <t>If have TDP data:</t>
+  </si>
+  <si>
+    <t>If have TP data:</t>
+  </si>
+  <si>
+    <t>Areal soil mass calculation (kg/m2), Msoil_m2</t>
+  </si>
+  <si>
+    <t>This sheet provides some simple aides to parameterising the model. It is not read in to the model</t>
+  </si>
+  <si>
+    <t>M:\Working\NewModel\ModelInputs\Tar_AvMetData_1981-2010.csv</t>
+  </si>
+  <si>
+    <t>M:\Working\NewModel\ModelInputs\obs_csvs\Coull_9amDailyMeanQ_oldRating.xlsx</t>
+  </si>
+  <si>
+    <t>M:\Working\NewModel\ModelInputs\obs_csvs\WholePeriod\TarChem_R4_SS-P.xlsx</t>
+  </si>
+  <si>
+    <t>Only required if Dynamic_erodibility is set to 'y' in Setup parameters.</t>
+  </si>
+  <si>
+    <t>Only required if Dynamic_erodibility is set to 'y' in Setup parameters. e.g. 1st of March. Conversion from Calendar day to Julian day, see e.g. http://landweb.nascom.nasa.gov/browse/calendar.html</t>
+  </si>
+  <si>
+    <t>File paths for work desktop:</t>
+  </si>
+  <si>
+    <t>File paths for work laptop:</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Text; format 'yyyy-mm-dd'</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Text: cal or other (case sensitive)</t>
+  </si>
+  <si>
+    <t>Text: y or n (case sensitive)</t>
+  </si>
+  <si>
+    <t>output_fpath</t>
+  </si>
+  <si>
+    <t>File path to folder for model output to be written to (graphs and csvs)</t>
+  </si>
+  <si>
+    <t>plot_TC</t>
+  </si>
+  <si>
+    <t>plot_R</t>
+  </si>
+  <si>
+    <t>Save a plot of simulated output from the terrestrial compartment?</t>
+  </si>
+  <si>
+    <t>Save a plot of simulated output from the stream reaches?</t>
+  </si>
+  <si>
+    <t>List of reaches to plot reach output for</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>R_vars_to_plot</t>
+  </si>
+  <si>
+    <t>List of instream variables to plot</t>
+  </si>
+  <si>
+    <t>Choose from: SS, TDP, PP, TP, Q</t>
+  </si>
+  <si>
+    <t>output_figtype</t>
+  </si>
+  <si>
+    <t>File type for output figures to be saved as</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>Choose from: eps, jpg, pdf, pgf, png, ps, raw, rgba, svg, tif</t>
+  </si>
+  <si>
+    <t>output_fig_dpi</t>
+  </si>
+  <si>
+    <t>Resolution required for figures, in dpi</t>
+  </si>
+  <si>
+    <t>Integer, e.g. 150, 300, 600</t>
+  </si>
+  <si>
+    <t>Integer, e.g. 1</t>
+  </si>
+  <si>
+    <t>M:\Working\NewModel\ModelOutputs\Figs</t>
+  </si>
+  <si>
+    <t>plot_snow</t>
+  </si>
+  <si>
+    <t>If snow module included, plot results?</t>
+  </si>
+  <si>
+    <t>plot_reaches</t>
+  </si>
+  <si>
+    <t>plot_obs_style</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>Choose from: line, point (case sensitive)</t>
+  </si>
+  <si>
+    <t>Either list desired reaches (e.g. 1,2,10), or enter the word 'all' (case sensitive)</t>
+  </si>
+  <si>
+    <t>Plot reach timeseries in black &amp; white or colour?</t>
+  </si>
+  <si>
+    <t>colour_option</t>
+  </si>
+  <si>
+    <t>colour</t>
+  </si>
+  <si>
+    <t>Choose from: b&amp;w, colour</t>
+  </si>
+  <si>
+    <t>logy_list</t>
+  </si>
+  <si>
+    <t>SS, PP, TP</t>
+  </si>
+  <si>
+    <t>save_stats_csv</t>
+  </si>
+  <si>
+    <t>Output a csv of model performance statistics?</t>
+  </si>
+  <si>
+    <t>save_output_csvs</t>
+  </si>
+  <si>
+    <t>Output csvs of model results?</t>
+  </si>
+  <si>
+    <t>How should the instream chemistry observations be plotted, as a line or as points? Discharge plotted as a line</t>
+  </si>
+  <si>
+    <t>2004-01-01</t>
+  </si>
+  <si>
+    <t>f_quick</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>For reach plots, provide a list of variables for which y-axis is log-transformed</t>
+  </si>
+  <si>
+    <t>2004-12-31</t>
+  </si>
+  <si>
     <t>a_Q</t>
   </si>
   <si>
     <t>b_Q</t>
-  </si>
-  <si>
-    <t>Qg0_init</t>
-  </si>
-  <si>
-    <t>Qr0_init</t>
-  </si>
-  <si>
-    <t>E_Q</t>
-  </si>
-  <si>
-    <t>k_EQ</t>
-  </si>
-  <si>
-    <t>TDPeff</t>
-  </si>
-  <si>
-    <t>TDPg</t>
-  </si>
-  <si>
-    <t>E_PP</t>
-  </si>
-  <si>
-    <t>Msoil_m2</t>
-  </si>
-  <si>
-    <t>Q_m3/s</t>
-  </si>
-  <si>
-    <t>TDP_kg/day</t>
-  </si>
-  <si>
-    <t>fraction as TDP</t>
-  </si>
-  <si>
-    <t>TP_kg/day</t>
-  </si>
-  <si>
-    <t>Template for calculating daily sewage fluxes to the stream (kg P/day as PP or TDP), from known effluent discharge and P concentration</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Soil water time constant</t>
-  </si>
-  <si>
-    <t>Proportion of precipitation that contributes to quick flow</t>
-  </si>
-  <si>
-    <t>PET reduction factor</t>
-  </si>
-  <si>
-    <t>km2</t>
-  </si>
-  <si>
-    <t>Catchment area</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>degrees</t>
-  </si>
-  <si>
-    <t>kg/day</t>
-  </si>
-  <si>
-    <t>Reach length</t>
-  </si>
-  <si>
-    <t>Reach effluent TDP inputs</t>
-  </si>
-  <si>
-    <t>Baseflow index</t>
-  </si>
-  <si>
-    <t>Groundwater time constant</t>
-  </si>
-  <si>
-    <t>mm/d</t>
-  </si>
-  <si>
-    <t>Minimum groundwater flow</t>
-  </si>
-  <si>
-    <t>1/m3</t>
-  </si>
-  <si>
-    <t>Gradient of stream velocity-discharge relationship</t>
-  </si>
-  <si>
-    <t>Exponent of stream velocity-discharge relationship</t>
-  </si>
-  <si>
-    <t>Initial groundwater flow</t>
-  </si>
-  <si>
-    <t>Initial in-stream flow</t>
-  </si>
-  <si>
-    <t>m3/s</t>
-  </si>
-  <si>
-    <t>kg/m2</t>
-  </si>
-  <si>
-    <t>Soil mass per m2</t>
-  </si>
-  <si>
-    <t>Soil bulk density</t>
-  </si>
-  <si>
-    <t>Soil depth</t>
-  </si>
-  <si>
-    <t>Soil mass/m2</t>
-  </si>
-  <si>
-    <t>kg/m3</t>
-  </si>
-  <si>
-    <t>cm</t>
-  </si>
-  <si>
-    <t>Particulate P enrichment factor</t>
-  </si>
-  <si>
-    <t>Groundwater TDP concentration</t>
-  </si>
-  <si>
-    <t>Instream entrainment factor</t>
-  </si>
-  <si>
-    <t>Instream entrainment non-linear coefficient</t>
-  </si>
-  <si>
-    <t>Soil field capacity</t>
-  </si>
-  <si>
-    <t>mm/kg soil</t>
-  </si>
-  <si>
-    <t>Terrestrial sediment delivery non-linear coefficient</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Hydrology</t>
-  </si>
-  <si>
-    <t>Dissolved P</t>
-  </si>
-  <si>
-    <t>Particulate P</t>
-  </si>
-  <si>
-    <t>Sediment</t>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>T_s</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Initial soil water EPC0, in mg/l</t>
-  </si>
-  <si>
-    <t>Semi-natural fixed</t>
-  </si>
-  <si>
-    <t>NC</t>
-  </si>
-  <si>
-    <t>f_NC_Ar</t>
-  </si>
-  <si>
-    <t>f_NC_IG</t>
-  </si>
-  <si>
-    <t>f_NC_S</t>
-  </si>
-  <si>
-    <t>Proportion of newly-converted SN (from agricultural). If have newly-converted IG or Ar, this must be 0</t>
-  </si>
-  <si>
-    <t>Proportion of newly-converted arable land (from SN). If f_NC_S&gt;0, this must be 0</t>
-  </si>
-  <si>
-    <t>Proportion of newly-converted IG (from SN). If f_NC_S&gt;0, this must be 0</t>
-  </si>
-  <si>
-    <t>Semi-natural fixed at 0. Newly-converted value could be negative if have net uptake.</t>
-  </si>
-  <si>
-    <t>Net annual P input to the soil (may be negative if have more uptake than input)</t>
-  </si>
-  <si>
-    <t>A value only needs to be supplied when the model is run in validation mode. In calibration mode, it is calculated within the model and output as Kf</t>
-  </si>
-  <si>
-    <t>Proportion of arable land, excluding any newly-converted from SN</t>
-  </si>
-  <si>
-    <t>Proportion of improved grassland, excluding any newly-converted from SN</t>
-  </si>
-  <si>
-    <t>Proportion of semi-natural and other low soil-P land, excluding any newly-converted from agricultural</t>
-  </si>
-  <si>
-    <t>S_Ar</t>
-  </si>
-  <si>
-    <t>S_IG</t>
-  </si>
-  <si>
-    <t>Mean slope of arable land in the sub-catchment</t>
-  </si>
-  <si>
-    <t>Mean slope of improved grassland in the sub-catchment</t>
-  </si>
-  <si>
-    <t>Mean slope of semi-natural land in the sub-catchment</t>
-  </si>
-  <si>
-    <t>Scaling factor for soil yield to the stream</t>
-  </si>
-  <si>
-    <t>m s2/kg</t>
-  </si>
-  <si>
-    <t>K_erosion</t>
-  </si>
-  <si>
-    <t>T/ha</t>
-  </si>
-  <si>
-    <t>Inherent soil erodibility, averaged for soils over the sub-catchment. Derived e.g. from http://esdac.jrc.ec.europa.eu/themes/soil-erodibility-europe</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>d_maxE_spr</t>
-  </si>
-  <si>
-    <t>d_maxE_aut</t>
-  </si>
-  <si>
-    <t>Day of the year when soil erodibility is at its maximum for spring-sown crops</t>
-  </si>
-  <si>
-    <t>Day of the year when soil erodibility is at its maximum for autumn-sown crops</t>
-  </si>
-  <si>
-    <t>Reach slope (ideally length-weighted)</t>
-  </si>
-  <si>
-    <t>Incorporates connectivity. May therefore need to change per sub-catchment</t>
-  </si>
-  <si>
-    <t>Vegetation cover factor, describing ratio between long-term erosion under the land use class, compared to under bare soil of the same soil type, slope, etc. Sourced from (R)USLE literature.</t>
-  </si>
-  <si>
-    <t>C_cover</t>
-  </si>
-  <si>
-    <t>f_spr</t>
-  </si>
-  <si>
-    <t>Proportion spring-sown crops make to total arable land area (assume rest is autumn-sown)</t>
-  </si>
-  <si>
-    <t>Sed_measures</t>
-  </si>
-  <si>
-    <t>S_SN</t>
-  </si>
-  <si>
-    <t>Reduction in load of sediment delivered to the stream (proportion; 0-1) due to management measures, e.g. buffer strips, filter fences, conservation tillage practices, etc.)</t>
-  </si>
-  <si>
-    <t>Phosphorus sorption coefficient (gradient of linear relationship between labile P and TDP concentration)</t>
-  </si>
-  <si>
-    <t>Initial total soil P content. If you only have 'labile P' data, calculate this using your assumed ratio for the connection between total and labile soil P masses ('k_labile' in 'constant' parameters)</t>
-  </si>
-  <si>
-    <t>Snow</t>
-  </si>
-  <si>
-    <t>D_snow_0</t>
-  </si>
-  <si>
-    <t>Initial snow depth in the catchment</t>
-  </si>
-  <si>
-    <t>f_DDSM</t>
-  </si>
-  <si>
-    <t>mm/(degree-day deg C)</t>
-  </si>
-  <si>
-    <t>Degree-day factor for snow melt</t>
-  </si>
-  <si>
-    <t>metdata_fpath</t>
-  </si>
-  <si>
-    <t>File path to input meteorological data file</t>
-  </si>
-  <si>
-    <t>Qobsdata_fpath</t>
-  </si>
-  <si>
-    <t>File path to discharge observations</t>
-  </si>
-  <si>
-    <t>chemObsData_fpath</t>
-  </si>
-  <si>
-    <t>File path to chemistry observations</t>
-  </si>
-  <si>
-    <t>C:\Users\lj40184\Documents\GitHub\enviro_mod_notes\notebooks\ModelInputs\Tar_AvMetData_1981-2010.csv</t>
-  </si>
-  <si>
-    <t>C:\Users\lj40184\Documents\GitHub\enviro_mod_notes\notebooks\ModelInputs\obs_csvs\Coull_9amDailyMeanQ_oldRating.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\lj40184\Documents\GitHub\enviro_mod_notes\notebooks\ModelInputs\obs_csvs\WholePeriod\TarChem_R4_SS-P.xlsx</t>
-  </si>
-  <si>
-    <t>run_mode</t>
-  </si>
-  <si>
-    <t>One of 'cal', 'other'. Determines whether the soil sorption coefficient, Kf, is calculated (calibration period) or read in as a parameter</t>
-  </si>
-  <si>
-    <t>cal</t>
-  </si>
-  <si>
-    <t>Simulation start date</t>
-  </si>
-  <si>
-    <t>Simulation end date. Format 'yyyy-mm-dd'</t>
-  </si>
-  <si>
-    <t>st_dt</t>
-  </si>
-  <si>
-    <t>end_dt</t>
-  </si>
-  <si>
-    <t>n_SC</t>
-  </si>
-  <si>
-    <t>Number of sub-catchments</t>
-  </si>
-  <si>
-    <t>Dynamic_EPC0</t>
-  </si>
-  <si>
-    <t>Calculate a dynamic soil water EPC0 (the equilibrium P concentration of zero sorption), so that it  varies with labile P content, or keep constant?</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>Dynamic_effluent_inputs</t>
-  </si>
-  <si>
-    <t>Dynamic_terrestrialP_inputs</t>
-  </si>
-  <si>
-    <t>Dynamic_erodibility</t>
-  </si>
-  <si>
-    <t>Calculate within-year variability in soil erodibility due to crop management practices?</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>Not yet implemented</t>
-  </si>
-  <si>
-    <t>inc_snowmelt</t>
-  </si>
-  <si>
-    <t>Include the snow accumulation and melt sub-module?</t>
-  </si>
-  <si>
-    <t>TDP_mg/l</t>
-  </si>
-  <si>
-    <t>TP_mg/l</t>
-  </si>
-  <si>
-    <t>If have TDP data:</t>
-  </si>
-  <si>
-    <t>If have TP data:</t>
-  </si>
-  <si>
-    <t>Areal soil mass calculation (kg/m2), Msoil_m2</t>
-  </si>
-  <si>
-    <t>This sheet provides some simple aides to parameterising the model. It is not read in to the model</t>
-  </si>
-  <si>
-    <t>M:\Working\NewModel\ModelInputs\Tar_AvMetData_1981-2010.csv</t>
-  </si>
-  <si>
-    <t>M:\Working\NewModel\ModelInputs\obs_csvs\Coull_9amDailyMeanQ_oldRating.xlsx</t>
-  </si>
-  <si>
-    <t>M:\Working\NewModel\ModelInputs\obs_csvs\WholePeriod\TarChem_R4_SS-P.xlsx</t>
-  </si>
-  <si>
-    <t>Only required if Dynamic_erodibility is set to 'y' in Setup parameters.</t>
-  </si>
-  <si>
-    <t>Only required if Dynamic_erodibility is set to 'y' in Setup parameters. e.g. 1st of March. Conversion from Calendar day to Julian day, see e.g. http://landweb.nascom.nasa.gov/browse/calendar.html</t>
-  </si>
-  <si>
-    <t>File paths for work desktop:</t>
-  </si>
-  <si>
-    <t>File paths for work laptop:</t>
-  </si>
-  <si>
-    <t>Format</t>
-  </si>
-  <si>
-    <t>Text; format 'yyyy-mm-dd'</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Text: cal or other (case sensitive)</t>
-  </si>
-  <si>
-    <t>Text: y or n (case sensitive)</t>
-  </si>
-  <si>
-    <t>output_fpath</t>
-  </si>
-  <si>
-    <t>File path to folder for model output to be written to (graphs and csvs)</t>
-  </si>
-  <si>
-    <t>plot_TC</t>
-  </si>
-  <si>
-    <t>plot_R</t>
-  </si>
-  <si>
-    <t>Save a plot of simulated output from the terrestrial compartment?</t>
-  </si>
-  <si>
-    <t>Save a plot of simulated output from the stream reaches?</t>
-  </si>
-  <si>
-    <t>List of reaches to plot reach output for</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>R_vars_to_plot</t>
-  </si>
-  <si>
-    <t>List of instream variables to plot</t>
-  </si>
-  <si>
-    <t>Choose from: SS, TDP, PP, TP, Q</t>
-  </si>
-  <si>
-    <t>output_figtype</t>
-  </si>
-  <si>
-    <t>File type for output figures to be saved as</t>
-  </si>
-  <si>
-    <t>png</t>
-  </si>
-  <si>
-    <t>Choose from: eps, jpg, pdf, pgf, png, ps, raw, rgba, svg, tif</t>
-  </si>
-  <si>
-    <t>output_fig_dpi</t>
-  </si>
-  <si>
-    <t>Resolution required for figures, in dpi</t>
-  </si>
-  <si>
-    <t>Integer, e.g. 150, 300, 600</t>
-  </si>
-  <si>
-    <t>Integer, e.g. 1</t>
-  </si>
-  <si>
-    <t>M:\Working\NewModel\ModelOutputs\Figs</t>
-  </si>
-  <si>
-    <t>plot_snow</t>
-  </si>
-  <si>
-    <t>If snow module included, plot results?</t>
-  </si>
-  <si>
-    <t>plot_reaches</t>
-  </si>
-  <si>
-    <t>plot_obs_style</t>
-  </si>
-  <si>
-    <t>line</t>
-  </si>
-  <si>
-    <t>Choose from: line, point (case sensitive)</t>
-  </si>
-  <si>
-    <t>Either list desired reaches (e.g. 1,2,10), or enter the word 'all' (case sensitive)</t>
-  </si>
-  <si>
-    <t>Plot reach timeseries in black &amp; white or colour?</t>
-  </si>
-  <si>
-    <t>colour_option</t>
-  </si>
-  <si>
-    <t>colour</t>
-  </si>
-  <si>
-    <t>Choose from: b&amp;w, colour</t>
-  </si>
-  <si>
-    <t>logy_list</t>
-  </si>
-  <si>
-    <t>SS, PP, TP</t>
-  </si>
-  <si>
-    <t>save_stats_csv</t>
-  </si>
-  <si>
-    <t>Output a csv of model performance statistics?</t>
-  </si>
-  <si>
-    <t>save_output_csvs</t>
-  </si>
-  <si>
-    <t>Output csvs of model results?</t>
-  </si>
-  <si>
-    <t>How should the instream chemistry observations be plotted, as a line or as points? Discharge plotted as a line</t>
-  </si>
-  <si>
-    <t>2004-01-01</t>
-  </si>
-  <si>
-    <t>f_quick</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>2005-12-31</t>
-  </si>
-  <si>
-    <t>For reach plots, provide a list of variables for which y-axis is log-transformed</t>
   </si>
 </sst>
 </file>
@@ -1517,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,355 +1535,355 @@
         <v>0</v>
       </c>
       <c r="B1" s="105" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C1" s="106" t="s">
         <v>26</v>
       </c>
       <c r="D1" s="105" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="108" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B2" s="109" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C2" s="102" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D2" s="99" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="108" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" s="109" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C3" s="102" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D3" s="99" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="108" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B4" s="109" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C4" s="102" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D4" s="99" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="108" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B5" s="109" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C5" s="102" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D5" s="99" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="108" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="109" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="102" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="109" t="s">
-        <v>145</v>
-      </c>
-      <c r="C6" s="102" t="s">
-        <v>146</v>
-      </c>
       <c r="D6" s="99" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="108" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B7" s="109" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C7" s="102" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D7" s="99" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="108" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B8" s="109" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C8" s="103" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D8" s="99" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="108" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B9" s="109" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C9" s="103" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D9" s="99" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="108" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B10" s="109" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C10" s="102">
         <v>1</v>
       </c>
       <c r="D10" s="99" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="108" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B11" s="109" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C11" s="102" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D11" s="115" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="108" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B12" s="109" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C12" s="102" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D12" s="115" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="110" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B13" s="111"/>
       <c r="C13" s="101" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D13" s="112"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="110" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B14" s="111"/>
       <c r="C14" s="101" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D14" s="112"/>
     </row>
     <row r="15" spans="1:4" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="113" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B15" s="114" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C15" s="100" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D15" s="115" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="113" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B16" s="114" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C16" s="100" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D16" s="115" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="113" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B17" s="114" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C17" s="100" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D17" s="115" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="100" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="113" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18" s="114" t="s">
         <v>184</v>
       </c>
-      <c r="B18" s="114" t="s">
-        <v>186</v>
-      </c>
       <c r="C18" s="100" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D18" s="115" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="108" t="s">
+        <v>183</v>
+      </c>
+      <c r="B19" s="114" t="s">
         <v>185</v>
       </c>
-      <c r="B19" s="114" t="s">
-        <v>187</v>
-      </c>
       <c r="C19" s="102" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D19" s="115" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="108" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="99" t="s">
+        <v>192</v>
+      </c>
+      <c r="C20" s="102" t="s">
         <v>193</v>
       </c>
-      <c r="B20" s="99" t="s">
+      <c r="D20" s="116" t="s">
         <v>194</v>
-      </c>
-      <c r="C20" s="102" t="s">
-        <v>195</v>
-      </c>
-      <c r="D20" s="116" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="108" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B21" s="99" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C21" s="102">
         <v>300</v>
       </c>
       <c r="D21" s="99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="108" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B22" s="99" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C22" s="102" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D22" s="116" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="108" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" s="99" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" s="102" t="s">
+        <v>220</v>
+      </c>
+      <c r="D23" s="116" t="s">
         <v>190</v>
-      </c>
-      <c r="B23" s="99" t="s">
-        <v>191</v>
-      </c>
-      <c r="C23" s="102" t="s">
-        <v>222</v>
-      </c>
-      <c r="D23" s="116" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="108" t="s">
+        <v>203</v>
+      </c>
+      <c r="B24" s="109" t="s">
+        <v>217</v>
+      </c>
+      <c r="C24" s="102" t="s">
+        <v>204</v>
+      </c>
+      <c r="D24" s="116" t="s">
         <v>205</v>
-      </c>
-      <c r="B24" s="109" t="s">
-        <v>219</v>
-      </c>
-      <c r="C24" s="102" t="s">
-        <v>206</v>
-      </c>
-      <c r="D24" s="116" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="108" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" s="109" t="s">
+        <v>207</v>
+      </c>
+      <c r="C25" s="102" t="s">
+        <v>209</v>
+      </c>
+      <c r="D25" s="116" t="s">
         <v>210</v>
-      </c>
-      <c r="B25" s="109" t="s">
-        <v>209</v>
-      </c>
-      <c r="C25" s="102" t="s">
-        <v>211</v>
-      </c>
-      <c r="D25" s="116" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B26" s="117" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D26" s="118" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -1897,7 +1897,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1910,7 +1910,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" s="68" t="s">
         <v>0</v>
@@ -1919,7 +1919,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="68" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E1" s="67" t="s">
         <v>1</v>
@@ -1931,24 +1931,24 @@
         <v>3</v>
       </c>
       <c r="H1" s="69" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I1" s="69" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" s="75" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C2" s="75" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="75" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E2" s="76">
         <v>2</v>
@@ -1962,7 +1962,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="81" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" s="82" t="s">
         <v>8</v>
@@ -1971,7 +1971,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="82" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E3" s="83">
         <v>1100</v>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" s="59" t="s">
         <v>9</v>
@@ -1994,7 +1994,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E4" s="70">
         <v>10</v>
@@ -2007,12 +2007,12 @@
         <v>-3</v>
       </c>
       <c r="I4" s="61" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" s="64" t="s">
         <v>10</v>
@@ -2021,7 +2021,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="64" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E5" s="88">
         <v>0.12</v>
@@ -2032,21 +2032,21 @@
       <c r="G5" s="65"/>
       <c r="H5" s="73"/>
       <c r="I5" s="66" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B6" s="59" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C6" s="59" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E6" s="58">
         <v>0.2</v>
@@ -2062,16 +2062,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="63" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" s="64" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C7" s="64" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="64" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E7" s="63">
         <v>0</v>
@@ -2093,10 +2093,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E3:E5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,9 +2106,9 @@
     <col min="4" max="4" width="93.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" s="68" t="s">
         <v>0</v>
@@ -2117,32 +2117,32 @@
         <v>12</v>
       </c>
       <c r="D1" s="68" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E1" s="92">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B2" s="96" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="82" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" s="82" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E2" s="97">
         <v>51.7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="90" t="s">
         <v>22</v>
@@ -2151,15 +2151,15 @@
         <v>19</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E3" s="93">
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4" s="90" t="s">
         <v>21</v>
@@ -2168,15 +2168,15 @@
         <v>19</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E4" s="93">
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="90" t="s">
         <v>23</v>
@@ -2185,194 +2185,197 @@
         <v>19</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E5" s="93">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" s="90" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" s="59" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E6" s="93">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B7" s="90" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" s="59" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="59" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E7" s="93">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" s="90" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" s="59" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="59" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E8" s="93">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B9" s="90" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C9" s="59" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E9" s="93">
+        <v>1</v>
+      </c>
+      <c r="F9">
         <v>0.65</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10" s="90" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="59" t="s">
         <v>103</v>
-      </c>
-      <c r="C10" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="59" t="s">
-        <v>105</v>
       </c>
       <c r="E10" s="94">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B11" s="90" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="59" t="s">
         <v>104</v>
-      </c>
-      <c r="C11" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="59" t="s">
-        <v>106</v>
       </c>
       <c r="E11" s="94">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B12" s="90" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C12" s="59" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D12" s="59" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E12" s="94">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B13" s="91" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E13" s="98">
         <v>5000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="81" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14" s="96" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="82" t="s">
         <v>110</v>
-      </c>
-      <c r="C14" s="82" t="s">
-        <v>111</v>
-      </c>
-      <c r="D14" s="82" t="s">
-        <v>112</v>
       </c>
       <c r="E14" s="97">
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B15" s="91" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="64" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D15" s="64" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E15" s="98">
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="63" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B16" s="91" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="64" t="s">
         <v>53</v>
-      </c>
-      <c r="D16" s="64" t="s">
-        <v>55</v>
       </c>
       <c r="E16" s="95">
         <v>0.26</v>
@@ -2388,8 +2391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2405,7 +2408,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>0</v>
@@ -2414,27 +2417,27 @@
         <v>12</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E1" s="28" t="s">
         <v>26</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E2" s="22">
         <v>0</v>
@@ -2443,16 +2446,16 @@
     </row>
     <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B3" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>132</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>134</v>
       </c>
       <c r="E3" s="25">
         <v>2.74</v>
@@ -2461,16 +2464,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C4" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E4" s="44">
         <v>1.4999999999999999E-2</v>
@@ -2479,7 +2482,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>5</v>
@@ -2488,7 +2491,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E5" s="33">
         <v>0.95</v>
@@ -2497,7 +2500,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>4</v>
@@ -2506,7 +2509,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E6" s="34">
         <v>290</v>
@@ -2515,7 +2518,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>27</v>
@@ -2524,7 +2527,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E7" s="33">
         <v>0.6</v>
@@ -2533,7 +2536,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B8" s="31" t="s">
         <v>28</v>
@@ -2542,7 +2545,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" s="34">
         <v>65</v>
@@ -2551,16 +2554,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E9" s="35">
         <v>0.4</v>
@@ -2569,16 +2572,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>30</v>
+        <v>223</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E10" s="35">
         <v>0.5</v>
@@ -2587,16 +2590,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>31</v>
+        <v>224</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E11" s="35">
         <v>0.5</v>
@@ -2605,16 +2608,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E12" s="35">
         <v>1</v>
@@ -2623,16 +2626,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E13" s="40">
         <v>1</v>
@@ -2641,16 +2644,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E14" s="46">
         <v>200</v>
@@ -2659,36 +2662,36 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E15" s="36">
         <v>3.2237299999999997E-5</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="39" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E16" s="47">
         <v>1.4999999999999999E-2</v>
@@ -2697,16 +2700,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17" s="49" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E17" s="50">
         <v>2</v>
@@ -2715,27 +2718,27 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B18" s="31" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E18" s="31">
         <v>30</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B19" s="31" t="s">
         <v>7</v>
@@ -2744,7 +2747,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E19" s="35">
         <v>1.2</v>
@@ -2753,56 +2756,56 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="52" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B20" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="53" t="s">
         <v>114</v>
-      </c>
-      <c r="C20" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="D20" s="53" t="s">
-        <v>116</v>
       </c>
       <c r="E20" s="53">
         <v>60</v>
       </c>
       <c r="F20" s="54" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B21" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="53" t="s">
         <v>115</v>
-      </c>
-      <c r="C21" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="D21" s="53" t="s">
-        <v>117</v>
       </c>
       <c r="E21" s="53">
         <v>304</v>
       </c>
       <c r="F21" s="55" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" s="31" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E22" s="34">
         <v>250</v>
@@ -2811,16 +2814,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" s="39" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E23" s="40">
         <v>1.7</v>
@@ -2856,28 +2859,28 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2894,24 +2897,24 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="D9" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2935,81 +2938,81 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B14" s="14">
         <v>1000</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B15" s="5">
         <v>20</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" s="17">
         <f>B14*B15/100</f>
         <v>200</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="57" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="57" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="57" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Amended bed sediment P content, plus minor alterations
Changed the P content of entrained bed sediments, so it reflects not
only the area of agricultural vs semi-natural land in the sub-catchment,
but also the inputs to the stream from the different land use classes.
E.g. if have no erosion from semi-natural land, then in-stream seds will
reflect arable seds. A simplification, but hopefully more realistic.

Also:
- Fixed small bug in the performance stats cell
- Changed initial Qg, so it is now calculated by the model rather than
being a user-supplied parameter (Qg0 = beta*Qr0)
- Graphs and stats now always displayed in the notebook, regardless of
whether they're saved to file
</commit_message>
<xml_diff>
--- a/notebooks/ModelInputs/parameters_v2.xlsx
+++ b/notebooks/ModelInputs/parameters_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="18195" windowHeight="11520" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="390" windowWidth="18195" windowHeight="11460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="227">
   <si>
     <t>Param</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Qg_min</t>
   </si>
   <si>
-    <t>Qg0_init</t>
-  </si>
-  <si>
     <t>Qr0_init</t>
   </si>
   <si>
@@ -203,9 +200,6 @@
     <t>Exponent of stream velocity-discharge relationship</t>
   </si>
   <si>
-    <t>Initial groundwater flow</t>
-  </si>
-  <si>
     <t>Initial in-stream flow</t>
   </si>
   <si>
@@ -278,9 +272,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Initial soil water EPC0, in mg/l</t>
-  </si>
-  <si>
     <t>Semi-natural fixed</t>
   </si>
   <si>
@@ -386,21 +377,12 @@
     <t>Proportion spring-sown crops make to total arable land area (assume rest is autumn-sown)</t>
   </si>
   <si>
-    <t>Sed_measures</t>
-  </si>
-  <si>
     <t>S_SN</t>
   </si>
   <si>
-    <t>Reduction in load of sediment delivered to the stream (proportion; 0-1) due to management measures, e.g. buffer strips, filter fences, conservation tillage practices, etc.)</t>
-  </si>
-  <si>
     <t>Phosphorus sorption coefficient (gradient of linear relationship between labile P and TDP concentration)</t>
   </si>
   <si>
-    <t>Initial total soil P content. If you only have 'labile P' data, calculate this using your assumed ratio for the connection between total and labile soil P masses ('k_labile' in 'constant' parameters)</t>
-  </si>
-  <si>
     <t>Snow</t>
   </si>
   <si>
@@ -680,9 +662,6 @@
     <t>f_quick</t>
   </si>
   <si>
-    <t>Q</t>
-  </si>
-  <si>
     <t>For reach plots, provide a list of variables for which y-axis is log-transformed</t>
   </si>
   <si>
@@ -693,6 +672,33 @@
   </si>
   <si>
     <t>b_Q</t>
+  </si>
+  <si>
+    <t>Initial soil water EPC0</t>
+  </si>
+  <si>
+    <t>soil_P_dataType</t>
+  </si>
+  <si>
+    <t>Is the input soil P data provided as total P or soil test P (STP)?</t>
+  </si>
+  <si>
+    <t>Text: total or STP</t>
+  </si>
+  <si>
+    <t>Initial total soil P content. If you only have 'labile P' data, calculate this using your assumed ratio for the connection between total and labile soil P masses</t>
+  </si>
+  <si>
+    <t>C_measures</t>
+  </si>
+  <si>
+    <t>Q, SS, PP</t>
+  </si>
+  <si>
+    <t>Reduction in load of sediment delivered to the stream (proportion; 0-1) due to management measures, e.g. buffer strips, filter fences, conservation tillage practices, etc.). E.g. 10% reduction in load due to measures would be 0.1</t>
+  </si>
+  <si>
+    <t>Soil P</t>
   </si>
 </sst>
 </file>
@@ -974,7 +980,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1080,9 +1086,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1093,18 +1096,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1160,9 +1151,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1187,15 +1175,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1212,6 +1191,54 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1515,375 +1542,389 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="102" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.85546875" style="102" customWidth="1"/>
-    <col min="3" max="3" width="40.42578125" style="102" customWidth="1"/>
-    <col min="4" max="4" width="53.5703125" style="102" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="102"/>
+    <col min="1" max="1" width="26.7109375" style="96" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" style="96" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" style="96" customWidth="1"/>
+    <col min="4" max="4" width="53.5703125" style="96" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="96"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="107" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
+    <row r="1" spans="1:4" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="106" t="s">
+      <c r="B1" s="99" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="105" t="s">
+      <c r="D1" s="99" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="102" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="103" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="96" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="94" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="102" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="103" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="96" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="94" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="102" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="103" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="96" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="94" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="102" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="103" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="108" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" s="109" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" s="102" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" s="99" t="s">
+      <c r="C5" s="96" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" s="94" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="102" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="103" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="96" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="94" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="102" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="103" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="96" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="94" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="102" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="103" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="97" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="94" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="102" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="103" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="97" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9" s="94" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="102" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="103" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="96">
+        <v>1</v>
+      </c>
+      <c r="D10" s="94" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="102" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="103" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="96" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="106" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="122" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="119" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" s="120" t="s">
+        <v>220</v>
+      </c>
+      <c r="C12" s="125" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="121" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="102" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="103" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="96" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="106" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="122" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="123" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="124"/>
+      <c r="C14" s="125" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" s="126"/>
+    </row>
+    <row r="15" spans="1:4" s="122" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="123" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="124"/>
+      <c r="C15" s="125" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="126"/>
+    </row>
+    <row r="16" spans="1:4" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="104" t="s">
+        <v>209</v>
+      </c>
+      <c r="B16" s="105" t="s">
+        <v>210</v>
+      </c>
+      <c r="C16" s="95" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" s="106" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="104" t="s">
+        <v>207</v>
+      </c>
+      <c r="B17" s="105" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" s="95" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="106" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="104" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" s="105" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="95" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" s="106" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="95" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="104" t="s">
+        <v>176</v>
+      </c>
+      <c r="B19" s="105" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" s="95" t="s">
+        <v>152</v>
+      </c>
+      <c r="D19" s="106" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="102" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="108" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" s="109" t="s">
-        <v>136</v>
-      </c>
-      <c r="C3" s="102" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" s="99" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="108" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4" s="109" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="102" t="s">
-        <v>170</v>
-      </c>
-      <c r="D4" s="99" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="108" t="s">
+      <c r="B20" s="105" t="s">
+        <v>179</v>
+      </c>
+      <c r="C20" s="96" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="106" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="102" t="s">
+        <v>185</v>
+      </c>
+      <c r="B21" s="94" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" s="96" t="s">
+        <v>187</v>
+      </c>
+      <c r="D21" s="107" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="102" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" s="94" t="s">
+        <v>190</v>
+      </c>
+      <c r="C22" s="96">
+        <v>300</v>
+      </c>
+      <c r="D22" s="94" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" s="94" t="s">
         <v>180</v>
       </c>
-      <c r="B5" s="109" t="s">
+      <c r="C23" s="96" t="s">
         <v>181</v>
       </c>
-      <c r="C5" s="102" t="s">
+      <c r="D23" s="107" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="102" t="s">
+        <v>182</v>
+      </c>
+      <c r="B24" s="94" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" s="96" t="s">
+        <v>224</v>
+      </c>
+      <c r="D24" s="107" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="102" t="s">
+        <v>197</v>
+      </c>
+      <c r="B25" s="103" t="s">
+        <v>211</v>
+      </c>
+      <c r="C25" s="96" t="s">
+        <v>198</v>
+      </c>
+      <c r="D25" s="107" t="s">
         <v>199</v>
       </c>
-      <c r="D5" s="99" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="108" t="s">
-        <v>142</v>
-      </c>
-      <c r="B6" s="109" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6" s="102" t="s">
-        <v>144</v>
-      </c>
-      <c r="D6" s="99" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="108" t="s">
-        <v>160</v>
-      </c>
-      <c r="B7" s="109" t="s">
-        <v>161</v>
-      </c>
-      <c r="C7" s="102" t="s">
-        <v>153</v>
-      </c>
-      <c r="D7" s="99" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="108" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" s="109" t="s">
-        <v>145</v>
-      </c>
-      <c r="C8" s="103" t="s">
-        <v>218</v>
-      </c>
-      <c r="D8" s="99" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="108" t="s">
-        <v>148</v>
-      </c>
-      <c r="B9" s="109" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="103" t="s">
-        <v>222</v>
-      </c>
-      <c r="D9" s="99" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="108" t="s">
-        <v>149</v>
-      </c>
-      <c r="B10" s="109" t="s">
-        <v>150</v>
-      </c>
-      <c r="C10" s="102">
-        <v>1</v>
-      </c>
-      <c r="D10" s="99" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="108" t="s">
-        <v>151</v>
-      </c>
-      <c r="B11" s="109" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" s="102" t="s">
-        <v>158</v>
-      </c>
-      <c r="D11" s="115" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="108" t="s">
-        <v>156</v>
-      </c>
-      <c r="B12" s="109" t="s">
-        <v>157</v>
-      </c>
-      <c r="C12" s="102" t="s">
-        <v>153</v>
-      </c>
-      <c r="D12" s="115" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="110" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" s="111"/>
-      <c r="C13" s="101" t="s">
-        <v>159</v>
-      </c>
-      <c r="D13" s="112"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="110" t="s">
-        <v>155</v>
-      </c>
-      <c r="B14" s="111"/>
-      <c r="C14" s="101" t="s">
-        <v>159</v>
-      </c>
-      <c r="D14" s="112"/>
-    </row>
-    <row r="15" spans="1:4" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="113" t="s">
-        <v>215</v>
-      </c>
-      <c r="B15" s="114" t="s">
-        <v>216</v>
-      </c>
-      <c r="C15" s="100" t="s">
-        <v>158</v>
-      </c>
-      <c r="D15" s="115" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="113" t="s">
-        <v>213</v>
-      </c>
-      <c r="B16" s="114" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="102" t="s">
+        <v>202</v>
+      </c>
+      <c r="B26" s="103" t="s">
+        <v>201</v>
+      </c>
+      <c r="C26" s="96" t="s">
+        <v>203</v>
+      </c>
+      <c r="D26" s="107" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="B27" s="108" t="s">
         <v>214</v>
       </c>
-      <c r="C16" s="100" t="s">
-        <v>158</v>
-      </c>
-      <c r="D16" s="115" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="100" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="113" t="s">
-        <v>200</v>
-      </c>
-      <c r="B17" s="114" t="s">
-        <v>201</v>
-      </c>
-      <c r="C17" s="100" t="s">
-        <v>158</v>
-      </c>
-      <c r="D17" s="115" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="100" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="113" t="s">
-        <v>182</v>
-      </c>
-      <c r="B18" s="114" t="s">
+      <c r="C27" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="D27" s="109" t="s">
         <v>184</v>
-      </c>
-      <c r="C18" s="100" t="s">
-        <v>158</v>
-      </c>
-      <c r="D18" s="115" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="108" t="s">
-        <v>183</v>
-      </c>
-      <c r="B19" s="114" t="s">
-        <v>185</v>
-      </c>
-      <c r="C19" s="102" t="s">
-        <v>158</v>
-      </c>
-      <c r="D19" s="115" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="108" t="s">
-        <v>191</v>
-      </c>
-      <c r="B20" s="99" t="s">
-        <v>192</v>
-      </c>
-      <c r="C20" s="102" t="s">
-        <v>193</v>
-      </c>
-      <c r="D20" s="116" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="108" t="s">
-        <v>195</v>
-      </c>
-      <c r="B21" s="99" t="s">
-        <v>196</v>
-      </c>
-      <c r="C21" s="102">
-        <v>300</v>
-      </c>
-      <c r="D21" s="99" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="108" t="s">
-        <v>202</v>
-      </c>
-      <c r="B22" s="99" t="s">
-        <v>186</v>
-      </c>
-      <c r="C22" s="102" t="s">
-        <v>187</v>
-      </c>
-      <c r="D22" s="116" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="108" t="s">
-        <v>188</v>
-      </c>
-      <c r="B23" s="99" t="s">
-        <v>189</v>
-      </c>
-      <c r="C23" s="102" t="s">
-        <v>220</v>
-      </c>
-      <c r="D23" s="116" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="108" t="s">
-        <v>203</v>
-      </c>
-      <c r="B24" s="109" t="s">
-        <v>217</v>
-      </c>
-      <c r="C24" s="102" t="s">
-        <v>204</v>
-      </c>
-      <c r="D24" s="116" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="108" t="s">
-        <v>208</v>
-      </c>
-      <c r="B25" s="109" t="s">
-        <v>207</v>
-      </c>
-      <c r="C25" s="102" t="s">
-        <v>209</v>
-      </c>
-      <c r="D25" s="116" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="B26" s="117" t="s">
-        <v>221</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>212</v>
-      </c>
-      <c r="D26" s="118" t="s">
-        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -1897,7 +1938,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,181 +1950,181 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="68" t="s">
+      <c r="A1" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="64" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="70" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="70" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="68" t="s">
+      <c r="E2" s="71">
         <v>2</v>
       </c>
-      <c r="G1" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="69" t="s">
-        <v>88</v>
-      </c>
-      <c r="I1" s="69" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="75" t="s">
+      <c r="F2" s="72">
+        <v>7</v>
+      </c>
+      <c r="G2" s="73"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="75"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="76" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="77" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="77" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="77" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" s="78">
+        <v>1100</v>
+      </c>
+      <c r="F3" s="79">
+        <v>900</v>
+      </c>
+      <c r="G3" s="80"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="82"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="53" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="65">
+        <v>10</v>
+      </c>
+      <c r="F4" s="57">
+        <v>0</v>
+      </c>
+      <c r="G4" s="55"/>
+      <c r="H4" s="67">
+        <v>-3</v>
+      </c>
+      <c r="I4" s="56" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>218</v>
+      </c>
+      <c r="E5" s="83">
+        <v>0.12</v>
+      </c>
+      <c r="F5" s="84">
+        <v>0</v>
+      </c>
+      <c r="G5" s="60"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="75" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="75" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="76">
-        <v>2</v>
-      </c>
-      <c r="F2" s="77">
-        <v>7</v>
-      </c>
-      <c r="G2" s="78"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="80"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="81" t="s">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="82" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="82" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="83">
-        <v>1100</v>
-      </c>
-      <c r="F3" s="84">
-        <v>900</v>
-      </c>
-      <c r="G3" s="85"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="87"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+      <c r="B6" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="53">
+        <v>0.2</v>
+      </c>
+      <c r="F6" s="54">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="G6" s="54">
+        <v>0.09</v>
+      </c>
+      <c r="H6" s="66"/>
+      <c r="I6" s="56"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="59" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="59" t="s">
-        <v>96</v>
-      </c>
-      <c r="E4" s="70">
-        <v>10</v>
-      </c>
-      <c r="F4" s="62">
+      <c r="B7" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="E7" s="58">
         <v>0</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="72">
-        <v>-3</v>
-      </c>
-      <c r="I4" s="61" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="64" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="64" t="s">
-        <v>86</v>
-      </c>
-      <c r="E5" s="88">
-        <v>0.12</v>
-      </c>
-      <c r="F5" s="89">
+      <c r="F7" s="59">
         <v>0</v>
       </c>
-      <c r="G5" s="65"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="66" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="59" t="s">
-        <v>118</v>
-      </c>
-      <c r="E6" s="58">
-        <v>0.2</v>
-      </c>
-      <c r="F6" s="59">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G6" s="59">
-        <v>0.09</v>
-      </c>
-      <c r="H6" s="71"/>
-      <c r="I6" s="61"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="63" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="C7" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="64" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="63">
+      <c r="G7" s="59">
         <v>0</v>
       </c>
-      <c r="F7" s="64">
-        <v>0</v>
-      </c>
-      <c r="G7" s="64">
-        <v>0</v>
-      </c>
-      <c r="H7" s="73"/>
-      <c r="I7" s="66"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2093,10 +2134,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B3" sqref="B3:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,278 +2147,275 @@
     <col min="4" max="4" width="93.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="76" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="92">
+        <v>51.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="85" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="88">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="85" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="88">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="88">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="85" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="85" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="85" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="88">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="85" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="85" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="85" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" s="89">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="85" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="110">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="86" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="93">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="111" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="70" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="112">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="68" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="68" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="68" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="96" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="82" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="97">
-        <v>51.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="90" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="59" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="93">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="90" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="59" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" s="93">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="90" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="59" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="93">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="B6" s="90" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="59" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" s="93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="90" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="59" t="s">
-        <v>94</v>
-      </c>
-      <c r="E7" s="93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="90" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="59" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="90" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="59" t="s">
-        <v>121</v>
-      </c>
-      <c r="E9" s="93">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="90" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="59" t="s">
+      <c r="B16" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="94">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="90" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="94">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="90" t="s">
-        <v>123</v>
-      </c>
-      <c r="C12" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="59" t="s">
-        <v>105</v>
-      </c>
-      <c r="E12" s="94">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="64" t="s">
+      <c r="D16" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="98">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="81" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="96" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="82" t="s">
-        <v>109</v>
-      </c>
-      <c r="D14" s="82" t="s">
-        <v>110</v>
-      </c>
-      <c r="E14" s="97">
-        <v>2.4E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="63" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" s="91" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" s="98">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" s="91" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="95">
+      <c r="E16" s="90">
         <v>0.26</v>
       </c>
     </row>
@@ -2389,10 +2427,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2408,7 +2446,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>0</v>
@@ -2417,27 +2455,27 @@
         <v>12</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="28" t="s">
         <v>26</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E2" s="22">
         <v>0</v>
@@ -2446,16 +2484,16 @@
     </row>
     <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E3" s="25">
         <v>2.74</v>
@@ -2464,16 +2502,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C4" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="44">
         <v>1.4999999999999999E-2</v>
@@ -2482,7 +2520,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>5</v>
@@ -2491,7 +2529,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="33">
         <v>0.95</v>
@@ -2500,7 +2538,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>4</v>
@@ -2509,7 +2547,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E6" s="34">
         <v>290</v>
@@ -2518,7 +2556,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>27</v>
@@ -2527,7 +2565,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="33">
         <v>0.6</v>
@@ -2536,7 +2574,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8" s="31" t="s">
         <v>28</v>
@@ -2545,7 +2583,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="34">
         <v>65</v>
@@ -2554,16 +2592,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="31" t="s">
         <v>56</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>57</v>
       </c>
       <c r="E9" s="35">
         <v>0.4</v>
@@ -2572,16 +2610,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C10" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="31" t="s">
         <v>58</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>59</v>
       </c>
       <c r="E10" s="35">
         <v>0.5</v>
@@ -2590,16 +2628,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="35">
         <v>0.5</v>
@@ -2607,228 +2645,210 @@
       <c r="F11" s="32"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="40">
+        <v>1</v>
+      </c>
+      <c r="F12" s="41"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="46">
+        <v>200</v>
+      </c>
+      <c r="F13" s="45"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="36">
+        <v>3.2237299999999997E-5</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="127">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F15" s="50"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B16" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="49">
+        <v>2</v>
+      </c>
+      <c r="F16" s="50"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="31">
         <v>30</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="35">
-        <v>1</v>
-      </c>
-      <c r="F12" s="32"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="40">
-        <v>1</v>
-      </c>
-      <c r="F13" s="41"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="46">
-        <v>200</v>
-      </c>
-      <c r="F14" s="45"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="E15" s="36">
-        <v>3.2237299999999997E-5</v>
-      </c>
-      <c r="F15" s="37" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="47">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F16" s="41"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="50">
-        <v>2</v>
-      </c>
-      <c r="F17" s="51"/>
+      <c r="F17" s="37" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>107</v>
+        <v>19</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="31">
-        <v>30</v>
-      </c>
-      <c r="F18" s="37" t="s">
-        <v>117</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E18" s="35">
+        <v>1.2</v>
+      </c>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C19" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="34">
+        <v>250</v>
+      </c>
+      <c r="F19" s="32"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="35">
-        <v>1.2</v>
-      </c>
-      <c r="F19" s="32"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="52" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="53" t="s">
+      <c r="D20" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="40">
+        <v>1.7</v>
+      </c>
+      <c r="F20" s="41"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="113" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="114" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="114" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="114" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="114">
+        <v>60</v>
+      </c>
+      <c r="F21" s="115" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="116" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="117" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="117" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="117" t="s">
         <v>112</v>
       </c>
-      <c r="C20" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="D20" s="53" t="s">
-        <v>114</v>
-      </c>
-      <c r="E20" s="53">
-        <v>60</v>
-      </c>
-      <c r="F20" s="54" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="52" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="53" t="s">
-        <v>115</v>
-      </c>
-      <c r="E21" s="53">
+      <c r="E22" s="117">
         <v>304</v>
       </c>
-      <c r="F21" s="55" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="34">
-        <v>250</v>
-      </c>
-      <c r="F22" s="32"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="40">
-        <v>1.7</v>
-      </c>
-      <c r="F23" s="41"/>
+      <c r="F22" s="118" t="s">
+        <v>165</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2859,28 +2879,28 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>38</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2897,24 +2917,24 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>38</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2938,81 +2958,81 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B14" s="14">
         <v>1000</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B15" s="5">
         <v>20</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B16" s="17">
         <f>B14*B15/100</f>
         <v>200</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
-        <v>168</v>
+      <c r="A19" s="51" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="56" t="s">
-        <v>169</v>
+      <c r="A20" s="51" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="56" t="s">
-        <v>170</v>
+      <c r="A21" s="51" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="57" t="s">
-        <v>139</v>
+      <c r="A24" s="52" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="57" t="s">
-        <v>140</v>
+      <c r="A25" s="52" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="57" t="s">
-        <v>141</v>
+      <c r="A26" s="52" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>